<commit_message>
Test resource refactor, GeneralSnippets.md
</commit_message>
<xml_diff>
--- a/documents/Leetcode-problems.xlsx
+++ b/documents/Leetcode-problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\java-algorithms\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F7B3BA-ADB9-4A3F-B76E-F5DE695CF6E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABECDD1-10A2-46A0-AF0D-973FEDD2B4F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="117">
   <si>
     <t>#</t>
   </si>
@@ -416,13 +416,148 @@
   </si>
   <si>
     <t>Hashtable</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock/</t>
+  </si>
+  <si>
+    <t>121. Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/linked-list-cycle/</t>
+  </si>
+  <si>
+    <t>141. Linked List Cycle</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/middle-of-the-linked-list/</t>
+  </si>
+  <si>
+    <t>876. Middle of the Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindrome-linked-list/</t>
+  </si>
+  <si>
+    <t>234. Palindrome Linked List</t>
+  </si>
+  <si>
+    <t>203. Remove Linked List Elements</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-linked-list-elements/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-duplicates-from-sorted-list/</t>
+  </si>
+  <si>
+    <t>83. Remove Duplicates from Sorted List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-linked-list/</t>
+  </si>
+  <si>
+    <t>206. Reverse Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-two-sorted-lists/</t>
+  </si>
+  <si>
+    <t>21. Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t>252. Meeting Rooms</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/meeting-rooms/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/peak-index-in-a-mountain-array/</t>
+  </si>
+  <si>
+    <t>852. Peak Index in a Mountain Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/average-of-levels-in-binary-tree/</t>
+  </si>
+  <si>
+    <t>637. Average of Levels in Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-depth-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>111. Minimum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/same-tree/</t>
+  </si>
+  <si>
+    <t>100. Same Tree</t>
+  </si>
+  <si>
+    <t>112. Path Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-sum/</t>
+  </si>
+  <si>
+    <t>104. Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-depth-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>543. Diameter of Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/diameter-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-two-binary-trees/</t>
+  </si>
+  <si>
+    <t>617. Merge Two Binary Trees</t>
+  </si>
+  <si>
+    <t>235. Lowest Common Ancestor of a Binary Search Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>572. Subtree of Another Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subtree-of-another-tree/</t>
+  </si>
+  <si>
+    <t>226. Invert Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/invert-binary-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/backspace-string-compare/</t>
+  </si>
+  <si>
+    <t>844. Backspace String Compare</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/index-pairs-of-a-string/</t>
+  </si>
+  <si>
+    <t>1065. Index Pairs of a String</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,6 +580,14 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -463,13 +606,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -756,17 +902,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -795,13 +941,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>ROW()-1</f>
+        <f t="shared" ref="A2:A50" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D2" t="s">
@@ -816,13 +962,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D3" t="s">
@@ -837,13 +983,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D4" t="s">
@@ -855,13 +1001,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D5" t="s">
@@ -873,13 +1019,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D6" t="s">
@@ -894,13 +1040,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>57</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D7" t="s">
@@ -915,13 +1061,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>69</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D8" t="s">
@@ -936,13 +1082,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D9" t="s">
@@ -957,13 +1103,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D10" t="s">
@@ -978,13 +1124,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D11" t="s">
@@ -999,13 +1145,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D12" t="s">
@@ -1020,13 +1166,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D13" t="s">
@@ -1041,13 +1187,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>66</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D14" t="s">
@@ -1059,13 +1205,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D15" t="s">
@@ -1080,13 +1226,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D16" t="s">
@@ -1101,13 +1247,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>65</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D17" t="s">
@@ -1122,13 +1268,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D18" t="s">
@@ -1143,13 +1289,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>45</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D19" t="s">
@@ -1161,13 +1307,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D20" t="s">
@@ -1182,13 +1328,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D21" t="s">
@@ -1203,13 +1349,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D22" t="s">
@@ -1221,13 +1367,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D23" t="s">
@@ -1242,13 +1388,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D24" t="s">
@@ -1263,13 +1409,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D25" t="s">
@@ -1284,13 +1430,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D26" t="s">
@@ -1305,13 +1451,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D27" t="s">
@@ -1322,6 +1468,420 @@
       </c>
       <c r="F27" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D39" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D42" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D44" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" t="s">
+        <v>74</v>
+      </c>
+      <c r="E45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" t="s">
+        <v>74</v>
+      </c>
+      <c r="E47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" t="s">
+        <v>74</v>
+      </c>
+      <c r="E48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D49" t="s">
+        <v>74</v>
+      </c>
+      <c r="E49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>116</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" t="s">
+        <v>74</v>
+      </c>
+      <c r="E50" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1335,7 +1895,7 @@
       <formula>NOT(ISERROR(SEARCH("Solved",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E1048576 E1">
+  <conditionalFormatting sqref="E51:E1048576 E1">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1349,9 +1909,34 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" xr:uid="{AF582801-8C82-417A-BC90-754A4A4A273A}"/>
+    <hyperlink ref="C17" r:id="rId2" xr:uid="{93D7B805-0AAA-43DB-A5FB-8A47AFB4955F}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{360E041F-B0DD-4BBB-99F0-FEC11C74DF66}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{46F9E010-CBE8-4A2E-9C23-1ED4BB1B1F4E}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{25A28752-23E4-47D8-A121-5D1EA00837E8}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{3D1DAB51-3975-4C63-8024-DE42B1A10551}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{A88D270B-DD4D-4B26-B375-EB9E13EFB360}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{8212B78A-A644-47F5-98D0-3B1A37A7D45E}"/>
+    <hyperlink ref="C7" r:id="rId9" xr:uid="{7B89EAC2-F6B4-4EED-B8C9-86966B3540C8}"/>
+    <hyperlink ref="C9" r:id="rId10" xr:uid="{2CF0B45E-39BB-45F0-B562-6F6A109D4AE6}"/>
+    <hyperlink ref="C11" r:id="rId11" xr:uid="{F74243B0-9456-44C6-A8F8-7D4BC0097062}"/>
+    <hyperlink ref="C12" r:id="rId12" xr:uid="{9E0E15EC-C7D6-453F-BB20-B4DC44E847C0}"/>
+    <hyperlink ref="C13" r:id="rId13" xr:uid="{24945E02-001F-4EC2-B305-690B333CF5A7}"/>
+    <hyperlink ref="C14" r:id="rId14" xr:uid="{8EF49D9C-E60B-4173-BA06-3A5CB4948092}"/>
+    <hyperlink ref="C15" r:id="rId15" xr:uid="{EF98E54E-BA3E-4059-8787-256C26698DF2}"/>
+    <hyperlink ref="C16" r:id="rId16" xr:uid="{AFC88B2F-E281-44A4-B755-AEEEDC044D4E}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{FCF2CE55-9407-4234-BD39-9931FA7929A1}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{7170FF64-A78A-4745-A928-41A075FBEF23}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{2D20E59F-FD49-4561-9516-026EFCBAC280}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{E5A16AE2-EC0D-480F-92C4-628BBB8DF98B}"/>
+    <hyperlink ref="C23" r:id="rId21" xr:uid="{0F5CC868-171D-4ACE-AACF-92490F0A235F}"/>
+    <hyperlink ref="C22" r:id="rId22" xr:uid="{31C5E189-B075-4CA9-8FDB-D7FC91DE6008}"/>
+    <hyperlink ref="C24" r:id="rId23" xr:uid="{E7A6C803-C0F3-449E-8D52-3A4D7325CA42}"/>
+    <hyperlink ref="C25" r:id="rId24" xr:uid="{1CF48142-F48F-4E72-871F-8481378F69C0}"/>
+    <hyperlink ref="C26" r:id="rId25" xr:uid="{EB055FA2-9D2F-4517-AFA3-73B30C885722}"/>
+    <hyperlink ref="C27" r:id="rId26" xr:uid="{ECDFD730-14FE-4C5A-8BC7-5C597D35FD39}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
+  <legacyDrawing r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IntMinHeap, ImplementQueueUsingStacks+ImplementStackUsingQueues (troll solutions)
</commit_message>
<xml_diff>
--- a/documents/Leetcode-problems.xlsx
+++ b/documents/Leetcode-problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\java-algorithms\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FAEF6C-526F-4BB2-ABC0-E6106BB5D1BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F065A53-5BCF-4838-BCC4-EA4CA98D4A37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="130">
   <si>
     <t>#</t>
   </si>
@@ -578,6 +578,18 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/number-of-islands/</t>
+  </si>
+  <si>
+    <t>225. Implement Stack using Queues</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-stack-using-queues/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-queue-using-stacks/</t>
+  </si>
+  <si>
+    <t>232. Implement Queue using Stacks</t>
   </si>
 </sst>
 </file>
@@ -931,14 +943,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -968,7 +980,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f t="shared" ref="A2:A54" si="0">ROW()-1</f>
+        <f t="shared" ref="A2:A56" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1993,10 +2005,46 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C55" s="1"/>
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D55" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="1"/>
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D56" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C57" s="1"/>
@@ -2024,7 +2072,7 @@
       <formula>NOT(ISERROR(SEARCH("Solved",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51:E1048576 E1">
+  <conditionalFormatting sqref="E51:E54 E1 E57:E1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
SQL Department Highest Salary
</commit_message>
<xml_diff>
--- a/documents/Leetcode-problems.xlsx
+++ b/documents/Leetcode-problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\java-algorithms\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303E1B3A-DD0F-44AE-8B96-7A939C6449AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E6E6EE-5703-4C67-80CF-EB6B6176EDCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="139">
   <si>
     <t>#</t>
   </si>
@@ -608,6 +608,15 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/palindrome-partitioning/</t>
+  </si>
+  <si>
+    <t>184. Department Highest Salary</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/department-highest-salary/</t>
+  </si>
+  <si>
+    <t>SQL</t>
   </si>
 </sst>
 </file>
@@ -961,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2119,7 +2128,24 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C60" s="1"/>
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D60" t="s">
+        <v>138</v>
+      </c>
+      <c r="E60" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C61" s="1"/>

</xml_diff>

<commit_message>
MiddleOfTheLinkedList, LinkedListCycle, LinkedListCycleII, NumberOfProvinces
</commit_message>
<xml_diff>
--- a/documents/Leetcode-problems.xlsx
+++ b/documents/Leetcode-problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\java-algorithms\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E6E6EE-5703-4C67-80CF-EB6B6176EDCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2552D1-050F-47E3-A913-CA256788C004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="144">
   <si>
     <t>#</t>
   </si>
@@ -617,6 +617,21 @@
   </si>
   <si>
     <t>SQL</t>
+  </si>
+  <si>
+    <t>142. Linked List Cycle II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/linked-list-cycle-ii/</t>
+  </si>
+  <si>
+    <t>Fast and slow pointers</t>
+  </si>
+  <si>
+    <t>287. Find the Duplicate Number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-the-duplicate-number/</t>
   </si>
 </sst>
 </file>
@@ -968,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1022,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f t="shared" ref="A2:A59" si="0">ROW()-1</f>
+        <f t="shared" ref="A2:A62" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1566,10 +1581,13 @@
         <v>75</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
+      </c>
+      <c r="F29" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1584,10 +1602,13 @@
         <v>77</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
+      </c>
+      <c r="F30" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1991,6 +2012,9 @@
       <c r="E52" t="s">
         <v>16</v>
       </c>
+      <c r="F52" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
@@ -2129,6 +2153,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="B60" t="s">
@@ -2148,7 +2173,43 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C61" s="1"/>
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>139</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D61" t="s">
+        <v>141</v>
+      </c>
+      <c r="E61" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>142</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D62" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F51" xr:uid="{C23B0BE7-B939-4F07-89D3-55931AE85EFC}">

</xml_diff>

<commit_message>
HappyNumber, PalindromeLinkedList, ReverseLinkedList, GeneralSnippets.md
</commit_message>
<xml_diff>
--- a/documents/Leetcode-problems.xlsx
+++ b/documents/Leetcode-problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\java-algorithms\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2552D1-050F-47E3-A913-CA256788C004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F42BEA-9F5B-483E-AC4E-0A9029BD5DE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="151">
   <si>
     <t>#</t>
   </si>
@@ -632,6 +632,27 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/find-the-duplicate-number/</t>
+  </si>
+  <si>
+    <t>In-place reversal of a linked list</t>
+  </si>
+  <si>
+    <t>202. Happy Number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/happy-number/</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try a solution with time O(n) &amp; space O(1) </t>
+  </si>
+  <si>
+    <t>16. 3Sum Closest</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/3sum-closest/</t>
   </si>
 </sst>
 </file>
@@ -670,12 +691,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -691,9 +718,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -983,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G55" sqref="G54:G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,13 +1025,13 @@
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1019,10 +1050,13 @@
       <c r="F1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f t="shared" ref="A2:A62" si="0">ROW()-1</f>
+        <f t="shared" ref="A2:A64" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1041,7 +1075,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1062,7 +1096,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1080,7 +1114,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1098,7 +1132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1119,7 +1153,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1140,7 +1174,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1161,7 +1195,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1182,7 +1216,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1203,7 +1237,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1224,7 +1258,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1245,7 +1279,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1266,7 +1300,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1284,7 +1318,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1305,7 +1339,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1326,7 +1360,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1347,7 +1381,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1368,25 +1402,26 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1407,7 +1442,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1428,7 +1463,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1446,7 +1481,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1467,7 +1502,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1488,7 +1523,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1509,7 +1544,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1530,7 +1565,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1551,7 +1586,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1569,7 +1604,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1590,7 +1625,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1611,25 +1646,31 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="31" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1641,10 +1682,13 @@
         <v>82</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="E32" t="s">
         <v>15</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1677,10 +1721,13 @@
         <v>85</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
+      </c>
+      <c r="F34" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2038,22 +2085,23 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="2">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -2208,6 +2256,63 @@
         <v>17</v>
       </c>
       <c r="E62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>145</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D64" t="s">
+        <v>141</v>
+      </c>
+      <c r="E64" t="s">
+        <v>15</v>
+      </c>
+      <c r="F64" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>149</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D65" t="s">
+        <v>31</v>
+      </c>
+      <c r="E65" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2217,12 +2322,12 @@
       <sortCondition descending="1" ref="D1"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="F1:F1048576">
+  <conditionalFormatting sqref="F59:F1048576 F1:F57 G31 G1">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Solved">
       <formula>NOT(ISERROR(SEARCH("Solved",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51:E54 E1 E57:E1048576">
+  <conditionalFormatting sqref="E51:E54 E1 E57 E59:E1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
GraphValidTree, RemoveDuplicatesFromSortedList (crap solution)
</commit_message>
<xml_diff>
--- a/documents/Leetcode-problems.xlsx
+++ b/documents/Leetcode-problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\java-algorithms\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F42BEA-9F5B-483E-AC4E-0A9029BD5DE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918EBA55-5821-43E2-8043-2AB57A3EDEF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="156">
   <si>
     <t>#</t>
   </si>
@@ -653,6 +653,21 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/3sum-closest/</t>
+  </si>
+  <si>
+    <t>1971. Find if Path Exists in Graph</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-if-path-exists-in-graph/</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
+    <t>261. Graph Valid Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/graph-valid-tree/</t>
   </si>
 </sst>
 </file>
@@ -691,7 +706,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -701,6 +716,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,13 +739,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1014,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G55" sqref="G54:G55"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,7 +1079,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f t="shared" ref="A2:A64" si="0">ROW()-1</f>
+        <f t="shared" ref="A2:A66" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1692,22 +1715,23 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="6">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D33" t="s">
-        <v>74</v>
-      </c>
-      <c r="E33" t="s">
-        <v>15</v>
-      </c>
+      <c r="D33" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="6"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
@@ -2313,6 +2337,41 @@
         <v>31</v>
       </c>
       <c r="E65" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>151</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D66" t="s">
+        <v>153</v>
+      </c>
+      <c r="E66" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>154</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D67" t="s">
+        <v>121</v>
+      </c>
+      <c r="E67" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fast & slow pointers, BFS, DFS (failed attempt)
</commit_message>
<xml_diff>
--- a/documents/Leetcode-problems.xlsx
+++ b/documents/Leetcode-problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\java-algorithms\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9120E7-94D1-42C2-9D31-4F13BD7C2B16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76715606-967A-4B89-A0E0-CECBEF384264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Problems" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Problems!$A$1:$F$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Problems!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
     <author>downvoteit</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{B4F66DAE-58B9-4F7E-A52C-8A7B47507561}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{F5DF3227-E733-4162-B3C9-E2FE6EEAE87D}">
       <text>
         <r>
           <rPr>
@@ -47,8 +47,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
+            <charset val="1"/>
           </rPr>
           <t>downvoteit:</t>
         </r>
@@ -57,15 +56,15 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Return if left + right == target else left++/right--</t>
+Return if left + right == target else left++/right--
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{D3AFA7D9-C2E2-4797-A432-9EDB8FD81622}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{D3AFA7D9-C2E2-4797-A432-9EDB8FD81622}">
       <text>
         <r>
           <rPr>
@@ -91,7 +90,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{08703EE3-B838-4B83-A249-ECC104E9F69F}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{B655BBA3-B037-4E4D-AA35-A7EC7D40AC70}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>downvoteit:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+Add all to set, traverse the array (for), if set.contains(n -1) is false then while set.contains(n+next) increament the next, Math.max(maxLen, curLen)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{08703EE3-B838-4B83-A249-ECC104E9F69F}">
       <text>
         <r>
           <rPr>
@@ -117,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{9E9D3493-0E7D-48D9-81B6-F0FEF0B669AB}">
+    <comment ref="B38" authorId="0" shapeId="0" xr:uid="{9E9D3493-0E7D-48D9-81B6-F0FEF0B669AB}">
       <text>
         <r>
           <rPr>
@@ -143,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{7EB3A81C-A645-48D5-9C41-35C45B814EB6}">
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{7EB3A81C-A645-48D5-9C41-35C45B814EB6}">
       <text>
         <r>
           <rPr>
@@ -169,38 +194,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{B655BBA3-B037-4E4D-AA35-A7EC7D40AC70}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>downvoteit:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-Add all to set, traverse the array (for), if set.contains(n -1) is false then while set.contains(n+next) increament the next, Math.max(maxLen, curLen)</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="179">
   <si>
     <t>#</t>
   </si>
@@ -379,9 +378,6 @@
     <t>https://leetcode.com/problems/fizz-buzz/</t>
   </si>
   <si>
-    <t>Modulo</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/two-sum-ii-input-array-is-sorted/</t>
   </si>
   <si>
@@ -565,9 +561,6 @@
     <t>https://leetcode.com/problems/number-of-provinces/</t>
   </si>
   <si>
-    <t>Union-find</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/number-of-connected-components-in-an-undirected-graph/</t>
   </si>
   <si>
@@ -661,9 +654,6 @@
     <t>https://leetcode.com/problems/find-if-path-exists-in-graph/</t>
   </si>
   <si>
-    <t>BFS</t>
-  </si>
-  <si>
     <t>261. Graph Valid Tree</t>
   </si>
   <si>
@@ -709,14 +699,50 @@
     <t>54. Spiral Matrix</t>
   </si>
   <si>
-    <t>Matrix</t>
+    <t>Disjoint sets</t>
+  </si>
+  <si>
+    <t>Disjoint set</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>Breadth-first search</t>
+  </si>
+  <si>
+    <t>102. Binary Tree Level Order Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-level-order-traversal/</t>
+  </si>
+  <si>
+    <t>107. Binary Tree Level Order Traversal II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-level-order-traversal-ii/</t>
+  </si>
+  <si>
+    <t>Depth-first search</t>
+  </si>
+  <si>
+    <t>103. Binary Tree Zigzag Level Order Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-zigzag-level-order-traversal/</t>
+  </si>
+  <si>
+    <t>113. Path Sum II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-sum-ii/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -746,6 +772,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -781,13 +820,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
@@ -795,7 +833,42 @@
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1086,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,19 +1196,19 @@
         <v>36</v>
       </c>
       <c r="G1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f t="shared" ref="A2:A72" si="0">ROW()-1</f>
+        <f t="shared" ref="A2:A22" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
@@ -1174,16 +1247,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1192,16 +1268,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1210,13 +1289,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
@@ -1231,16 +1310,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
         <v>37</v>
@@ -1252,16 +1331,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
         <v>37</v>
@@ -1273,16 +1352,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>166</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
         <v>37</v>
@@ -1294,16 +1373,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>121</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>167</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
         <v>37</v>
@@ -1315,16 +1394,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>134</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>135</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>136</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
         <v>37</v>
@@ -1336,16 +1415,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>137</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>138</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
         <v>37</v>
@@ -1357,13 +1436,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>151</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>167</v>
       </c>
       <c r="E13" t="s">
         <v>16</v>
@@ -1378,13 +1457,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
@@ -1396,62 +1475,55 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E15" t="s">
         <v>16</v>
       </c>
-      <c r="F15" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" t="s">
-        <v>37</v>
-      </c>
+      <c r="E16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" t="s">
-        <v>37</v>
-      </c>
+      <c r="B17" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1459,39 +1531,35 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>52</v>
+        <v>130</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="2"/>
+      <c r="B19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1499,19 +1567,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1520,175 +1585,163 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>140</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>141</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="5">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" t="s">
-        <v>24</v>
+      <c r="B22" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="0"/>
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>147</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A24:A55" si="1">ROW()-1</f>
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>153</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>47</v>
+        <v>154</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>157</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>159</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>48</v>
+        <v>158</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>139</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f t="shared" si="0"/>
+      <c r="A26" s="5">
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" t="s">
-        <v>37</v>
-      </c>
+      <c r="B26" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f t="shared" si="0"/>
+      <c r="A27" s="5">
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" t="s">
-        <v>37</v>
-      </c>
+      <c r="B27" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" si="0"/>
+      <c r="A28" s="5">
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" t="s">
-        <v>15</v>
-      </c>
+      <c r="B28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>141</v>
+        <v>168</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
@@ -1699,17 +1752,17 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D30" t="s">
-        <v>141</v>
+        <v>70</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1719,142 +1772,144 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <f t="shared" si="0"/>
+      <c r="A31">
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>148</v>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>2</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="D32" t="s">
-        <v>141</v>
+        <v>3</v>
       </c>
       <c r="E32" t="s">
         <v>15</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
-        <f t="shared" si="0"/>
+      <c r="A33">
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="6"/>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
       </c>
       <c r="F34" t="s">
         <v>37</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="D35" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
+      </c>
+      <c r="F35" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D36" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="E36" t="s">
         <v>15</v>
+      </c>
+      <c r="F36" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
+        <v>6</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="E37" t="s">
         <v>15</v>
@@ -1865,254 +1920,299 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="D38" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
+      </c>
+      <c r="F38" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="D39" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
+      </c>
+      <c r="F39" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="D40" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="E40" t="s">
         <v>15</v>
+      </c>
+      <c r="F40" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="D41" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
+      </c>
+      <c r="F41" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
       <c r="D42" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
+      </c>
+      <c r="F42" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="D43" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
+      </c>
+      <c r="F43" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="D44" t="s">
-        <v>74</v>
+        <v>139</v>
       </c>
       <c r="E44" t="s">
         <v>15</v>
+      </c>
+      <c r="F44" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="D45" t="s">
-        <v>74</v>
+        <v>139</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
       </c>
+      <c r="F45" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <f t="shared" si="0"/>
+      <c r="A46" s="5">
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B46" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D46" t="s">
-        <v>74</v>
-      </c>
-      <c r="E46" t="s">
-        <v>15</v>
+      <c r="B46" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="D47" t="s">
-        <v>74</v>
+        <v>139</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
       </c>
+      <c r="F47" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <f t="shared" si="0"/>
+      <c r="A48" s="5">
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B48" t="s">
-        <v>35</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" t="s">
-        <v>74</v>
-      </c>
-      <c r="E48" t="s">
-        <v>15</v>
+      <c r="B48" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="D49" t="s">
-        <v>74</v>
+        <v>142</v>
       </c>
       <c r="E49" t="s">
         <v>15</v>
+      </c>
+      <c r="F49" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="D50" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="E50" t="s">
         <v>15</v>
+      </c>
+      <c r="F50" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D51" t="s">
-        <v>33</v>
+        <v>157</v>
       </c>
       <c r="E51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F51" t="s">
         <v>37</v>
@@ -2120,20 +2220,20 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D52" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="E52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F52" t="s">
         <v>37</v>
@@ -2141,270 +2241,258 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="D53" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="E53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
-        <f t="shared" si="0"/>
+      <c r="A54">
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F54" s="2"/>
+      <c r="B54" t="s">
+        <v>35</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D54" t="s">
+        <v>31</v>
+      </c>
+      <c r="E54" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>127</v>
+        <v>71</v>
       </c>
       <c r="D55" t="s">
-        <v>160</v>
+        <v>73</v>
       </c>
       <c r="E55" t="s">
         <v>15</v>
-      </c>
-      <c r="F55" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A56:A77" si="2">ROW()-1</f>
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="D56" t="s">
-        <v>160</v>
+        <v>73</v>
       </c>
       <c r="E56" t="s">
         <v>15</v>
-      </c>
-      <c r="F56" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="D57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="D58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E58" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F58" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>134</v>
+        <v>95</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="D59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>137</v>
+        <v>96</v>
       </c>
       <c r="D60" t="s">
-        <v>138</v>
+        <v>73</v>
       </c>
       <c r="E60" t="s">
-        <v>16</v>
-      </c>
-      <c r="F60" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <f t="shared" si="0"/>
+      <c r="A61" s="5">
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="B61" t="s">
-        <v>139</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D61" t="s">
-        <v>141</v>
-      </c>
-      <c r="E61" t="s">
-        <v>16</v>
-      </c>
-      <c r="F61" t="s">
-        <v>37</v>
-      </c>
+      <c r="B61" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>142</v>
+        <v>100</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>143</v>
+        <v>101</v>
       </c>
       <c r="D62" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="E62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="6">
-        <f t="shared" si="0"/>
+      <c r="A63">
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
-      <c r="B63" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F63" s="6"/>
+      <c r="B63" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D63" t="s">
+        <v>73</v>
+      </c>
+      <c r="E63" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>145</v>
+        <v>105</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="D64" t="s">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="E64" t="s">
         <v>15</v>
-      </c>
-      <c r="F64" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>149</v>
+        <v>106</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>150</v>
+        <v>107</v>
       </c>
       <c r="D65" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="E65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>151</v>
+        <v>108</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="D66" t="s">
-        <v>153</v>
+        <v>73</v>
       </c>
       <c r="E66" t="s">
         <v>15</v>
@@ -2412,56 +2500,53 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>154</v>
+        <v>110</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
       <c r="D67" t="s">
-        <v>121</v>
+        <v>73</v>
       </c>
       <c r="E67" t="s">
-        <v>16</v>
-      </c>
-      <c r="F67" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>156</v>
+        <v>35</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="D68" t="s">
-        <v>160</v>
+        <v>73</v>
       </c>
       <c r="E68" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
       <c r="D69" t="s">
-        <v>160</v>
+        <v>73</v>
       </c>
       <c r="E69" t="s">
         <v>15</v>
@@ -2469,73 +2554,168 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>162</v>
+        <v>115</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="D70" t="s">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="E70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="6">
-        <f t="shared" si="0"/>
+      <c r="A71">
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="B71" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F71" s="6"/>
+      <c r="B71" t="s">
+        <v>149</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D71" t="s">
+        <v>169</v>
+      </c>
+      <c r="E71" t="s">
+        <v>15</v>
+      </c>
+      <c r="F71"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="6">
-        <f t="shared" si="0"/>
+      <c r="A72">
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
-      <c r="B72" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D72" s="6" t="s">
+      <c r="B72" t="s">
+        <v>156</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D72" t="s">
+        <v>157</v>
+      </c>
+      <c r="E72" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>149</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D73" t="s">
         <v>169</v>
       </c>
-      <c r="E72" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F72" s="6"/>
+      <c r="E73" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>170</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D74" t="s">
+        <v>169</v>
+      </c>
+      <c r="E74" t="s">
+        <v>16</v>
+      </c>
+      <c r="F74" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="2"/>
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>172</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D75" t="s">
+        <v>169</v>
+      </c>
+      <c r="E75" t="s">
+        <v>16</v>
+      </c>
+      <c r="F75" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D76" t="s">
+        <v>169</v>
+      </c>
+      <c r="E76" t="s">
+        <v>16</v>
+      </c>
+      <c r="F76" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="5">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F77" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F51" xr:uid="{C23B0BE7-B939-4F07-89D3-55931AE85EFC}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F27">
-      <sortCondition descending="1" ref="D1"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="F59:F1048576 F1:F57 G31 G1">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Solved">
+  <autoFilter ref="A1:G1" xr:uid="{3809B7C5-5E24-49BB-A9E7-8AEF2B5426FA}"/>
+  <conditionalFormatting sqref="F59:F73 F1:F57 G22 G1 F76 F78:F1048576">
+    <cfRule type="containsText" dxfId="6" priority="13" operator="containsText" text="Solved">
       <formula>NOT(ISERROR(SEARCH("Solved",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51:E54 E1 E57 E59:E1048576">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="E51:E54 E1 E57 E59:E73 E76 E78:E1048576">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0"/>
@@ -2546,41 +2726,115 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",G34)))</formula>
+  <conditionalFormatting sqref="G46">
+    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",G46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G48">
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",G48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F74">
+    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F74)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E74">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F58">
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F75">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F75)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E75">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F77">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F77)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E77">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1" xr:uid="{AF582801-8C82-417A-BC90-754A4A4A273A}"/>
-    <hyperlink ref="C17" r:id="rId2" xr:uid="{93D7B805-0AAA-43DB-A5FB-8A47AFB4955F}"/>
+    <hyperlink ref="C32" r:id="rId1" xr:uid="{AF582801-8C82-417A-BC90-754A4A4A273A}"/>
+    <hyperlink ref="C36" r:id="rId2" xr:uid="{93D7B805-0AAA-43DB-A5FB-8A47AFB4955F}"/>
     <hyperlink ref="C2" r:id="rId3" xr:uid="{360E041F-B0DD-4BBB-99F0-FEC11C74DF66}"/>
     <hyperlink ref="C3" r:id="rId4" xr:uid="{46F9E010-CBE8-4A2E-9C23-1ED4BB1B1F4E}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{25A28752-23E4-47D8-A121-5D1EA00837E8}"/>
-    <hyperlink ref="C4" r:id="rId6" xr:uid="{3D1DAB51-3975-4C63-8024-DE42B1A10551}"/>
-    <hyperlink ref="C5" r:id="rId7" xr:uid="{A88D270B-DD4D-4B26-B375-EB9E13EFB360}"/>
-    <hyperlink ref="C8" r:id="rId8" xr:uid="{8212B78A-A644-47F5-98D0-3B1A37A7D45E}"/>
-    <hyperlink ref="C7" r:id="rId9" xr:uid="{7B89EAC2-F6B4-4EED-B8C9-86966B3540C8}"/>
-    <hyperlink ref="C9" r:id="rId10" xr:uid="{2CF0B45E-39BB-45F0-B562-6F6A109D4AE6}"/>
-    <hyperlink ref="C11" r:id="rId11" xr:uid="{F74243B0-9456-44C6-A8F8-7D4BC0097062}"/>
-    <hyperlink ref="C12" r:id="rId12" xr:uid="{9E0E15EC-C7D6-453F-BB20-B4DC44E847C0}"/>
-    <hyperlink ref="C13" r:id="rId13" xr:uid="{24945E02-001F-4EC2-B305-690B333CF5A7}"/>
-    <hyperlink ref="C14" r:id="rId14" xr:uid="{8EF49D9C-E60B-4173-BA06-3A5CB4948092}"/>
-    <hyperlink ref="C15" r:id="rId15" xr:uid="{EF98E54E-BA3E-4059-8787-256C26698DF2}"/>
-    <hyperlink ref="C16" r:id="rId16" xr:uid="{AFC88B2F-E281-44A4-B755-AEEEDC044D4E}"/>
-    <hyperlink ref="C18" r:id="rId17" xr:uid="{FCF2CE55-9407-4234-BD39-9931FA7929A1}"/>
-    <hyperlink ref="C19" r:id="rId18" xr:uid="{7170FF64-A78A-4745-A928-41A075FBEF23}"/>
-    <hyperlink ref="C20" r:id="rId19" xr:uid="{2D20E59F-FD49-4561-9516-026EFCBAC280}"/>
-    <hyperlink ref="C21" r:id="rId20" xr:uid="{E5A16AE2-EC0D-480F-92C4-628BBB8DF98B}"/>
-    <hyperlink ref="C23" r:id="rId21" xr:uid="{0F5CC868-171D-4ACE-AACF-92490F0A235F}"/>
-    <hyperlink ref="C22" r:id="rId22" xr:uid="{31C5E189-B075-4CA9-8FDB-D7FC91DE6008}"/>
-    <hyperlink ref="C24" r:id="rId23" xr:uid="{E7A6C803-C0F3-449E-8D52-3A4D7325CA42}"/>
-    <hyperlink ref="C25" r:id="rId24" xr:uid="{1CF48142-F48F-4E72-871F-8481378F69C0}"/>
-    <hyperlink ref="C26" r:id="rId25" xr:uid="{EB055FA2-9D2F-4517-AFA3-73B30C885722}"/>
-    <hyperlink ref="C27" r:id="rId26" xr:uid="{ECDFD730-14FE-4C5A-8BC7-5C597D35FD39}"/>
+    <hyperlink ref="C4" r:id="rId5" xr:uid="{25A28752-23E4-47D8-A121-5D1EA00837E8}"/>
+    <hyperlink ref="C54" r:id="rId6" xr:uid="{3D1DAB51-3975-4C63-8024-DE42B1A10551}"/>
+    <hyperlink ref="C14" r:id="rId7" xr:uid="{A88D270B-DD4D-4B26-B375-EB9E13EFB360}"/>
+    <hyperlink ref="C30" r:id="rId8" xr:uid="{8212B78A-A644-47F5-98D0-3B1A37A7D45E}"/>
+    <hyperlink ref="C29" r:id="rId9" xr:uid="{7B89EAC2-F6B4-4EED-B8C9-86966B3540C8}"/>
+    <hyperlink ref="C31" r:id="rId10" xr:uid="{2CF0B45E-39BB-45F0-B562-6F6A109D4AE6}"/>
+    <hyperlink ref="C33" r:id="rId11" xr:uid="{F74243B0-9456-44C6-A8F8-7D4BC0097062}"/>
+    <hyperlink ref="C34" r:id="rId12" xr:uid="{9E0E15EC-C7D6-453F-BB20-B4DC44E847C0}"/>
+    <hyperlink ref="C5" r:id="rId13" xr:uid="{24945E02-001F-4EC2-B305-690B333CF5A7}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{8EF49D9C-E60B-4173-BA06-3A5CB4948092}"/>
+    <hyperlink ref="C6" r:id="rId15" xr:uid="{EF98E54E-BA3E-4059-8787-256C26698DF2}"/>
+    <hyperlink ref="C35" r:id="rId16" xr:uid="{AFC88B2F-E281-44A4-B755-AEEEDC044D4E}"/>
+    <hyperlink ref="C37" r:id="rId17" xr:uid="{FCF2CE55-9407-4234-BD39-9931FA7929A1}"/>
+    <hyperlink ref="C16" r:id="rId18" xr:uid="{7170FF64-A78A-4745-A928-41A075FBEF23}"/>
+    <hyperlink ref="C38" r:id="rId19" xr:uid="{2D20E59F-FD49-4561-9516-026EFCBAC280}"/>
+    <hyperlink ref="C39" r:id="rId20" xr:uid="{E5A16AE2-EC0D-480F-92C4-628BBB8DF98B}"/>
+    <hyperlink ref="C40" r:id="rId21" xr:uid="{0F5CC868-171D-4ACE-AACF-92490F0A235F}"/>
+    <hyperlink ref="C28" r:id="rId22" xr:uid="{31C5E189-B075-4CA9-8FDB-D7FC91DE6008}"/>
+    <hyperlink ref="C41" r:id="rId23" xr:uid="{E7A6C803-C0F3-449E-8D52-3A4D7325CA42}"/>
+    <hyperlink ref="C42" r:id="rId24" xr:uid="{1CF48142-F48F-4E72-871F-8481378F69C0}"/>
+    <hyperlink ref="C7" r:id="rId25" xr:uid="{EB055FA2-9D2F-4517-AFA3-73B30C885722}"/>
+    <hyperlink ref="C43" r:id="rId26" xr:uid="{ECDFD730-14FE-4C5A-8BC7-5C597D35FD39}"/>
+    <hyperlink ref="C46" r:id="rId27" xr:uid="{C6BE8D11-FA44-4BC5-873A-F1E866EC28B5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
-  <legacyDrawing r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
+  <legacyDrawing r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
3 DFS questions, project refactor by patterns, test fixes, cleaning
</commit_message>
<xml_diff>
--- a/documents/Leetcode-problems.xlsx
+++ b/documents/Leetcode-problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\java-algorithms\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76715606-967A-4B89-A0E0-CECBEF384264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59C7F6E-3FD9-4AF0-988D-01EBA8DA4565}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <author>downvoteit</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{F5DF3227-E733-4162-B3C9-E2FE6EEAE87D}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{9E9D3493-0E7D-48D9-81B6-F0FEF0B669AB}">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>downvoteit:</t>
         </r>
@@ -56,15 +57,67 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
-Return if left + right == target else left++/right--
-</t>
+Modified binary search, return first if greater than last or smaller that first, else is an == statement, while loop to continue on duplicates and an if to break on array end</t>
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{D3AFA7D9-C2E2-4797-A432-9EDB8FD81622}">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{7EB3A81C-A645-48D5-9C41-35C45B814EB6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>downvoteit:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+Standard iterative binary search</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{08703EE3-B838-4B83-A249-ECC104E9F69F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>downvoteit:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+for i the array, add sum, if less than 0 reset to zero, Math.max(maxSum, curSum)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="0" shapeId="0" xr:uid="{D3AFA7D9-C2E2-4797-A432-9EDB8FD81622}">
       <text>
         <r>
           <rPr>
@@ -90,7 +143,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{B655BBA3-B037-4E4D-AA35-A7EC7D40AC70}">
+    <comment ref="B56" authorId="0" shapeId="0" xr:uid="{F5DF3227-E733-4162-B3C9-E2FE6EEAE87D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>downvoteit:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Return if left + right == target else left++/right--
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B66" authorId="0" shapeId="0" xr:uid="{B655BBA3-B037-4E4D-AA35-A7EC7D40AC70}">
       <text>
         <r>
           <rPr>
@@ -116,90 +194,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{08703EE3-B838-4B83-A249-ECC104E9F69F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>downvoteit:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-for i the array, add sum, if less than 0 reset to zero, Math.max(maxSum, curSum)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B38" authorId="0" shapeId="0" xr:uid="{9E9D3493-0E7D-48D9-81B6-F0FEF0B669AB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>downvoteit:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-Modified binary search, return first if greater than last or smaller that first, else is an == statement, while loop to continue on duplicates and an if to break on array end</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{7EB3A81C-A645-48D5-9C41-35C45B814EB6}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>downvoteit:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-Standard iterative binary search</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="187">
   <si>
     <t>#</t>
   </si>
@@ -702,9 +702,6 @@
     <t>Disjoint sets</t>
   </si>
   <si>
-    <t>Disjoint set</t>
-  </si>
-  <si>
     <t>Simulation</t>
   </si>
   <si>
@@ -736,6 +733,33 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/path-sum-ii/</t>
+  </si>
+  <si>
+    <t>101. Symmetric Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/symmetric-tree/</t>
+  </si>
+  <si>
+    <t>144. Binary Tree Preorder Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-preorder-traversal/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-inorder-traversal/</t>
+  </si>
+  <si>
+    <t>94. Binary Tree Inorder Traversal</t>
+  </si>
+  <si>
+    <t>145. Binary Tree Postorder Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-postorder-traversal/</t>
+  </si>
+  <si>
+    <t>String</t>
   </si>
 </sst>
 </file>
@@ -820,7 +844,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -828,12 +852,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -880,6 +933,106 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1159,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,80 +1354,75 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f t="shared" ref="A2:A22" si="0">ROW()-1</f>
+        <f>ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>183</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>182</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>173</v>
       </c>
       <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <f>ROW()-1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>37</v>
+      <c r="F4" s="5"/>
+      <c r="G4" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -1285,20 +1433,20 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>139</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
         <v>37</v>
@@ -1306,20 +1454,20 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
         <v>37</v>
@@ -1327,62 +1475,62 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="0"/>
+      <c r="A9" s="4">
+        <f>ROW()-1</f>
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D9" t="s">
-        <v>166</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
-        <v>37</v>
+      <c r="B9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>167</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
         <v>37</v>
@@ -1390,62 +1538,56 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="D11" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
       </c>
-      <c r="F11" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>152</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>167</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F13" t="s">
         <v>37</v>
@@ -1453,379 +1595,396 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>173</v>
       </c>
       <c r="E15" t="s">
         <v>16</v>
       </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="A16">
+        <f>ROW()-1</f>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>ROW()-1</f>
         <v>16</v>
       </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="2"/>
+      <c r="B17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="D18" t="s">
         <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>166</v>
       </c>
       <c r="E19" t="s">
         <v>16</v>
       </c>
+      <c r="F19" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="D20" t="s">
         <v>73</v>
       </c>
       <c r="E20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <f>ROW()-1</f>
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>140</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" t="s">
-        <v>16</v>
-      </c>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <f t="shared" si="0"/>
+      <c r="A22">
+        <f>ROW()-1</f>
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="4" t="s">
-        <v>146</v>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>64</v>
+        <f>ROW()-1</f>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>147</v>
+        <v>27</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>148</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" ref="A24:A55" si="1">ROW()-1</f>
+        <f>ROW()-1</f>
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="D24" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="E24" t="s">
         <v>16</v>
       </c>
+      <c r="F24" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f t="shared" si="1"/>
+      <c r="A25" s="2">
+        <f>ROW()-1</f>
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>159</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="B25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
-        <f t="shared" si="1"/>
+      <c r="A26">
+        <f>ROW()-1</f>
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="5"/>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
-        <f t="shared" si="1"/>
+      <c r="A27">
+        <f>ROW()-1</f>
         <v>26</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="5"/>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <f t="shared" si="1"/>
+      <c r="A28">
+        <f>ROW()-1</f>
         <v>27</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="5"/>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>159</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>58</v>
+        <v>158</v>
       </c>
       <c r="D29" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>166</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F30" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>55</v>
+        <v>141</v>
       </c>
       <c r="D32" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E32" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D33" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E33" t="s">
         <v>15</v>
@@ -1836,20 +1995,20 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>151</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>54</v>
+        <v>152</v>
       </c>
       <c r="D34" t="s">
-        <v>3</v>
+        <v>166</v>
       </c>
       <c r="E34" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F34" t="s">
         <v>37</v>
@@ -1857,80 +2016,77 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
-      </c>
-      <c r="F35" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="E36" t="s">
         <v>15</v>
       </c>
-      <c r="F36" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <f t="shared" si="1"/>
+      <c r="A37" s="4">
+        <f>ROW()-1</f>
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" t="s">
-        <v>37</v>
+      <c r="B37" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>127</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>60</v>
+        <v>126</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>157</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
@@ -1941,17 +2097,17 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="D39" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
@@ -1962,38 +2118,35 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="D40" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="E40" t="s">
         <v>15</v>
-      </c>
-      <c r="F40" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
       <c r="D41" t="s">
-        <v>18</v>
+        <v>157</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
@@ -2004,17 +2157,17 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="D42" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
@@ -2025,94 +2178,86 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="D43" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
-      </c>
-      <c r="F43" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="D44" t="s">
-        <v>139</v>
+        <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F44" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <f t="shared" si="1"/>
+      <c r="A45" s="5">
+        <f>ROW()-1</f>
         <v>44</v>
       </c>
-      <c r="B45" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D45" t="s">
-        <v>139</v>
-      </c>
-      <c r="E45" t="s">
-        <v>15</v>
-      </c>
-      <c r="F45" t="s">
-        <v>37</v>
-      </c>
+      <c r="B45" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
-        <f t="shared" si="1"/>
+      <c r="A46">
+        <f>ROW()-1</f>
         <v>45</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>146</v>
+      <c r="B46" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" t="s">
+        <v>142</v>
+      </c>
+      <c r="E46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>46</v>
       </c>
       <c r="B47" t="s">
@@ -2132,382 +2277,404 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
-        <f t="shared" si="1"/>
+      <c r="A48">
+        <f>ROW()-1</f>
         <v>47</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D48" s="5" t="s">
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f>ROW()-1</f>
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D49" t="s">
         <v>139</v>
       </c>
-      <c r="E48" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <f t="shared" si="1"/>
+      <c r="E49" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <f>ROW()-1</f>
+        <v>49</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
+        <f>ROW()-1</f>
+        <v>50</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f>ROW()-1</f>
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f>ROW()-1</f>
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>149</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D53" t="s">
+        <v>168</v>
+      </c>
+      <c r="E53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" s="4"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f>ROW()-1</f>
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>134</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D54" t="s">
+        <v>136</v>
+      </c>
+      <c r="E54" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f>ROW()-1</f>
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
-        <v>85</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D49" t="s">
-        <v>142</v>
-      </c>
-      <c r="E49" t="s">
-        <v>15</v>
-      </c>
-      <c r="F49" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>91</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="D55" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f>ROW()-1</f>
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f>ROW()-1</f>
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D57" t="s">
         <v>33</v>
       </c>
-      <c r="E50" t="s">
-        <v>15</v>
-      </c>
-      <c r="F50" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>124</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D51" t="s">
-        <v>157</v>
-      </c>
-      <c r="E51" t="s">
-        <v>15</v>
-      </c>
-      <c r="F51" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <f t="shared" si="1"/>
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>127</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D52" t="s">
-        <v>157</v>
-      </c>
-      <c r="E52" t="s">
-        <v>15</v>
-      </c>
-      <c r="F52" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <f t="shared" si="1"/>
+      <c r="E57" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>64</v>
+      </c>
+      <c r="B58" t="s">
+        <v>147</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E58" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f>ROW()-1</f>
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D59" t="s">
+        <v>31</v>
+      </c>
+      <c r="E59" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f>ROW()-1</f>
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>184</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D60" t="s">
+        <v>173</v>
+      </c>
+      <c r="E60" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f>ROW()-1</f>
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>180</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D61" t="s">
+        <v>173</v>
+      </c>
+      <c r="E61" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f>ROW()-1</f>
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>137</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D62" t="s">
+        <v>139</v>
+      </c>
+      <c r="E62" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f>ROW()-1</f>
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" t="s">
+        <v>139</v>
+      </c>
+      <c r="E63" t="s">
+        <v>15</v>
+      </c>
+      <c r="F63" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f>ROW()-1</f>
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B53" t="s">
-        <v>143</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D53" t="s">
-        <v>139</v>
-      </c>
-      <c r="E53" t="s">
-        <v>15</v>
-      </c>
-      <c r="F53" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <f t="shared" si="1"/>
-        <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>35</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D54" t="s">
-        <v>31</v>
-      </c>
-      <c r="E54" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <f t="shared" si="1"/>
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="D64" t="s">
+        <v>17</v>
+      </c>
+      <c r="E64" t="s">
+        <v>15</v>
+      </c>
+      <c r="F64" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f>ROW()-1</f>
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D65" t="s">
+        <v>173</v>
+      </c>
+      <c r="E65" t="s">
+        <v>16</v>
+      </c>
+      <c r="F65" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f>ROW()-1</f>
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D66" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f>ROW()-1</f>
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
         <v>72</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D55" t="s">
-        <v>73</v>
-      </c>
-      <c r="E55" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <f t="shared" ref="A56:A77" si="2">ROW()-1</f>
-        <v>55</v>
-      </c>
-      <c r="B56" t="s">
-        <v>87</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D56" t="s">
-        <v>73</v>
-      </c>
-      <c r="E56" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <f t="shared" si="2"/>
-        <v>56</v>
-      </c>
-      <c r="B57" t="s">
-        <v>88</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D57" t="s">
-        <v>73</v>
-      </c>
-      <c r="E57" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <f t="shared" si="2"/>
-        <v>57</v>
-      </c>
-      <c r="B58" t="s">
-        <v>93</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D58" t="s">
-        <v>73</v>
-      </c>
-      <c r="E58" t="s">
-        <v>15</v>
-      </c>
-      <c r="F58" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <f t="shared" si="2"/>
-        <v>58</v>
-      </c>
-      <c r="B59" t="s">
-        <v>95</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D59" t="s">
-        <v>73</v>
-      </c>
-      <c r="E59" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <f t="shared" si="2"/>
-        <v>59</v>
-      </c>
-      <c r="B60" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D60" t="s">
-        <v>73</v>
-      </c>
-      <c r="E60" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
-        <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F61" s="5"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <f t="shared" si="2"/>
-        <v>61</v>
-      </c>
-      <c r="B62" t="s">
-        <v>100</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D62" t="s">
-        <v>73</v>
-      </c>
-      <c r="E62" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <f t="shared" si="2"/>
-        <v>62</v>
-      </c>
-      <c r="B63" t="s">
-        <v>102</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D63" t="s">
-        <v>73</v>
-      </c>
-      <c r="E63" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <f t="shared" si="2"/>
-        <v>63</v>
-      </c>
-      <c r="B64" t="s">
-        <v>105</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D64" t="s">
-        <v>73</v>
-      </c>
-      <c r="E64" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <f t="shared" si="2"/>
-        <v>64</v>
-      </c>
-      <c r="B65" t="s">
-        <v>106</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D65" t="s">
-        <v>73</v>
-      </c>
-      <c r="E65" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <f t="shared" si="2"/>
-        <v>65</v>
-      </c>
-      <c r="B66" t="s">
-        <v>108</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D66" t="s">
-        <v>73</v>
-      </c>
-      <c r="E66" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <f t="shared" si="2"/>
-        <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>110</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="D67" t="s">
         <v>73</v>
@@ -2516,52 +2683,57 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <f t="shared" si="2"/>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="5">
+        <f>ROW()-1</f>
         <v>67</v>
       </c>
-      <c r="B68" t="s">
-        <v>35</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D68" t="s">
-        <v>73</v>
-      </c>
-      <c r="E68" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <f t="shared" si="2"/>
+      <c r="B68" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <f>ROW()-1</f>
         <v>68</v>
       </c>
-      <c r="B69" t="s">
-        <v>113</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D69" t="s">
-        <v>73</v>
-      </c>
-      <c r="E69" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G69"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="D70" t="s">
         <v>73</v>
@@ -2570,95 +2742,94 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>149</v>
+        <v>62</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="D71" t="s">
-        <v>169</v>
+        <v>31</v>
       </c>
       <c r="E71" t="s">
-        <v>15</v>
-      </c>
-      <c r="F71"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="D72" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="E72" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="F72" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>149</v>
+        <v>115</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="D73" t="s">
-        <v>169</v>
+        <v>73</v>
       </c>
       <c r="E73" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>171</v>
+        <v>101</v>
       </c>
       <c r="D74" t="s">
-        <v>169</v>
+        <v>73</v>
       </c>
       <c r="E74" t="s">
-        <v>16</v>
-      </c>
-      <c r="F74" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D75" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E75" t="s">
         <v>16</v>
@@ -2667,19 +2838,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D76" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E76" t="s">
         <v>16</v>
@@ -2688,34 +2859,76 @@
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="5">
-        <f t="shared" si="2"/>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f>ROW()-1</f>
         <v>76</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C77" s="6" t="s">
+      <c r="B77" t="s">
         <v>178</v>
       </c>
-      <c r="D77" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F77" s="5"/>
+      <c r="C77" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D77" t="s">
+        <v>168</v>
+      </c>
+      <c r="E77" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f>ROW()-1</f>
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>97</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D78" t="s">
+        <v>73</v>
+      </c>
+      <c r="E78" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <f>ROW()-1</f>
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D79" t="s">
+        <v>18</v>
+      </c>
+      <c r="E79" t="s">
+        <v>15</v>
+      </c>
+      <c r="F79" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{3809B7C5-5E24-49BB-A9E7-8AEF2B5426FA}"/>
-  <conditionalFormatting sqref="F59:F73 F1:F57 G22 G1 F76 F78:F1048576">
-    <cfRule type="containsText" dxfId="6" priority="13" operator="containsText" text="Solved">
+  <autoFilter ref="A1:G1" xr:uid="{3809B7C5-5E24-49BB-A9E7-8AEF2B5426FA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G81">
+      <sortCondition descending="1" ref="B1"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="F57:F71 G21 G1 F74 F80:F1048576 F1:F55">
+    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="Solved">
       <formula>NOT(ISERROR(SEARCH("Solved",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51:E54 E1 E57 E59:E73 E76 E78:E1048576">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="E50:E53 E55 E1 E57:E71 E74 E80:E1048576">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0"/>
@@ -2726,23 +2939,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G46">
-    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",G46)))</formula>
+  <conditionalFormatting sqref="G45">
+    <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",G45)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G48">
-    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",G48)))</formula>
+  <conditionalFormatting sqref="G47">
+    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",G47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F74">
-    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F74)))</formula>
+  <conditionalFormatting sqref="F72">
+    <cfRule type="containsText" dxfId="19" priority="14" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F72)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="E72">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0"/>
@@ -2753,12 +2966,46 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F58">
-    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F58)))</formula>
+  <conditionalFormatting sqref="F56">
+    <cfRule type="containsText" dxfId="18" priority="12" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E58">
+  <conditionalFormatting sqref="E56">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F73">
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F73)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E73">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F75">
+    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F75)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E75">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2770,12 +3017,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F75">
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F75)))</formula>
+  <conditionalFormatting sqref="F76">
+    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F76)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E75">
+  <conditionalFormatting sqref="E76">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2787,13 +3034,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F77">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Solved">
+  <conditionalFormatting sqref="F77:F79">
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Solved">
       <formula>NOT(ISERROR(SEARCH("Solved",F77)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E77">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="E77:E79">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0"/>
@@ -2804,37 +3051,41 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C32" r:id="rId1" xr:uid="{AF582801-8C82-417A-BC90-754A4A4A273A}"/>
-    <hyperlink ref="C36" r:id="rId2" xr:uid="{93D7B805-0AAA-43DB-A5FB-8A47AFB4955F}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{360E041F-B0DD-4BBB-99F0-FEC11C74DF66}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{46F9E010-CBE8-4A2E-9C23-1ED4BB1B1F4E}"/>
-    <hyperlink ref="C4" r:id="rId5" xr:uid="{25A28752-23E4-47D8-A121-5D1EA00837E8}"/>
-    <hyperlink ref="C54" r:id="rId6" xr:uid="{3D1DAB51-3975-4C63-8024-DE42B1A10551}"/>
-    <hyperlink ref="C14" r:id="rId7" xr:uid="{A88D270B-DD4D-4B26-B375-EB9E13EFB360}"/>
-    <hyperlink ref="C30" r:id="rId8" xr:uid="{8212B78A-A644-47F5-98D0-3B1A37A7D45E}"/>
-    <hyperlink ref="C29" r:id="rId9" xr:uid="{7B89EAC2-F6B4-4EED-B8C9-86966B3540C8}"/>
-    <hyperlink ref="C31" r:id="rId10" xr:uid="{2CF0B45E-39BB-45F0-B562-6F6A109D4AE6}"/>
-    <hyperlink ref="C33" r:id="rId11" xr:uid="{F74243B0-9456-44C6-A8F8-7D4BC0097062}"/>
-    <hyperlink ref="C34" r:id="rId12" xr:uid="{9E0E15EC-C7D6-453F-BB20-B4DC44E847C0}"/>
-    <hyperlink ref="C5" r:id="rId13" xr:uid="{24945E02-001F-4EC2-B305-690B333CF5A7}"/>
-    <hyperlink ref="C15" r:id="rId14" xr:uid="{8EF49D9C-E60B-4173-BA06-3A5CB4948092}"/>
-    <hyperlink ref="C6" r:id="rId15" xr:uid="{EF98E54E-BA3E-4059-8787-256C26698DF2}"/>
-    <hyperlink ref="C35" r:id="rId16" xr:uid="{AFC88B2F-E281-44A4-B755-AEEEDC044D4E}"/>
-    <hyperlink ref="C37" r:id="rId17" xr:uid="{FCF2CE55-9407-4234-BD39-9931FA7929A1}"/>
-    <hyperlink ref="C16" r:id="rId18" xr:uid="{7170FF64-A78A-4745-A928-41A075FBEF23}"/>
-    <hyperlink ref="C38" r:id="rId19" xr:uid="{2D20E59F-FD49-4561-9516-026EFCBAC280}"/>
-    <hyperlink ref="C39" r:id="rId20" xr:uid="{E5A16AE2-EC0D-480F-92C4-628BBB8DF98B}"/>
-    <hyperlink ref="C40" r:id="rId21" xr:uid="{0F5CC868-171D-4ACE-AACF-92490F0A235F}"/>
-    <hyperlink ref="C28" r:id="rId22" xr:uid="{31C5E189-B075-4CA9-8FDB-D7FC91DE6008}"/>
-    <hyperlink ref="C41" r:id="rId23" xr:uid="{E7A6C803-C0F3-449E-8D52-3A4D7325CA42}"/>
-    <hyperlink ref="C42" r:id="rId24" xr:uid="{1CF48142-F48F-4E72-871F-8481378F69C0}"/>
-    <hyperlink ref="C7" r:id="rId25" xr:uid="{EB055FA2-9D2F-4517-AFA3-73B30C885722}"/>
-    <hyperlink ref="C43" r:id="rId26" xr:uid="{ECDFD730-14FE-4C5A-8BC7-5C597D35FD39}"/>
-    <hyperlink ref="C46" r:id="rId27" xr:uid="{C6BE8D11-FA44-4BC5-873A-F1E866EC28B5}"/>
+    <hyperlink ref="C22" r:id="rId1" xr:uid="{AF582801-8C82-417A-BC90-754A4A4A273A}"/>
+    <hyperlink ref="C39" r:id="rId2" xr:uid="{93D7B805-0AAA-43DB-A5FB-8A47AFB4955F}"/>
+    <hyperlink ref="C56" r:id="rId3" xr:uid="{360E041F-B0DD-4BBB-99F0-FEC11C74DF66}"/>
+    <hyperlink ref="C59" r:id="rId4" xr:uid="{46F9E010-CBE8-4A2E-9C23-1ED4BB1B1F4E}"/>
+    <hyperlink ref="C44" r:id="rId5" xr:uid="{25A28752-23E4-47D8-A121-5D1EA00837E8}"/>
+    <hyperlink ref="C2" r:id="rId6" xr:uid="{3D1DAB51-3975-4C63-8024-DE42B1A10551}"/>
+    <hyperlink ref="C71" r:id="rId7" xr:uid="{A88D270B-DD4D-4B26-B375-EB9E13EFB360}"/>
+    <hyperlink ref="C42" r:id="rId8" xr:uid="{8212B78A-A644-47F5-98D0-3B1A37A7D45E}"/>
+    <hyperlink ref="C27" r:id="rId9" xr:uid="{7B89EAC2-F6B4-4EED-B8C9-86966B3540C8}"/>
+    <hyperlink ref="C14" r:id="rId10" xr:uid="{2CF0B45E-39BB-45F0-B562-6F6A109D4AE6}"/>
+    <hyperlink ref="C23" r:id="rId11" xr:uid="{F74243B0-9456-44C6-A8F8-7D4BC0097062}"/>
+    <hyperlink ref="C28" r:id="rId12" xr:uid="{9E0E15EC-C7D6-453F-BB20-B4DC44E847C0}"/>
+    <hyperlink ref="C52" r:id="rId13" xr:uid="{24945E02-001F-4EC2-B305-690B333CF5A7}"/>
+    <hyperlink ref="C31" r:id="rId14" xr:uid="{8EF49D9C-E60B-4173-BA06-3A5CB4948092}"/>
+    <hyperlink ref="C5" r:id="rId15" xr:uid="{EF98E54E-BA3E-4059-8787-256C26698DF2}"/>
+    <hyperlink ref="C33" r:id="rId16" xr:uid="{AFC88B2F-E281-44A4-B755-AEEEDC044D4E}"/>
+    <hyperlink ref="C64" r:id="rId17" xr:uid="{FCF2CE55-9407-4234-BD39-9931FA7929A1}"/>
+    <hyperlink ref="C25" r:id="rId18" xr:uid="{7170FF64-A78A-4745-A928-41A075FBEF23}"/>
+    <hyperlink ref="C10" r:id="rId19" xr:uid="{2D20E59F-FD49-4561-9516-026EFCBAC280}"/>
+    <hyperlink ref="C13" r:id="rId20" xr:uid="{E5A16AE2-EC0D-480F-92C4-628BBB8DF98B}"/>
+    <hyperlink ref="C26" r:id="rId21" xr:uid="{0F5CC868-171D-4ACE-AACF-92490F0A235F}"/>
+    <hyperlink ref="C50" r:id="rId22" xr:uid="{31C5E189-B075-4CA9-8FDB-D7FC91DE6008}"/>
+    <hyperlink ref="C48" r:id="rId23" xr:uid="{E7A6C803-C0F3-449E-8D52-3A4D7325CA42}"/>
+    <hyperlink ref="C55" r:id="rId24" xr:uid="{1CF48142-F48F-4E72-871F-8481378F69C0}"/>
+    <hyperlink ref="C66" r:id="rId25" xr:uid="{EB055FA2-9D2F-4517-AFA3-73B30C885722}"/>
+    <hyperlink ref="C79" r:id="rId26" xr:uid="{ECDFD730-14FE-4C5A-8BC7-5C597D35FD39}"/>
+    <hyperlink ref="C37" r:id="rId27" xr:uid="{C6BE8D11-FA44-4BC5-873A-F1E866EC28B5}"/>
+    <hyperlink ref="C61" r:id="rId28" xr:uid="{BCF24D75-89DC-45DD-8C0B-B89E1D3DBFA4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
-  <legacyDrawing r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <legacyDrawing r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
3 sliding window problems, Leetcode-problems.xlsx
</commit_message>
<xml_diff>
--- a/documents/Leetcode-problems.xlsx
+++ b/documents/Leetcode-problems.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\java-algorithms\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CF14D2-E14B-4BAB-8377-6CC20502F35B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32FD085-ACD0-4B5B-ABE5-AAA9449D0233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="24600" windowHeight="11385" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Problems!$A$1:$G$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Problems!$A$1:$G$85</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,173 +33,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>downvoteit</author>
-  </authors>
-  <commentList>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{F5DF3227-E733-4162-B3C9-E2FE6EEAE87D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>downvoteit:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Return if left + right == target else left++/right--
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{D3AFA7D9-C2E2-4797-A432-9EDB8FD81622}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>downvoteit:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-minLen = Integet.MAX_VALUE, for with winEnd, add n to minLen, while winSum &gt;= target Math.min(minLen, winEnd - winStart + 1) &amp;&amp; substract winStart from winSum &amp;&amp; increment winStart</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{08703EE3-B838-4B83-A249-ECC104E9F69F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>downvoteit:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-for i the array, add sum, if less than 0 reset to zero, Math.max(maxSum, curSum)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B61" authorId="0" shapeId="0" xr:uid="{9E9D3493-0E7D-48D9-81B6-F0FEF0B669AB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>downvoteit:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-Modified binary search, return first if greater than last or smaller that first, else is an == statement, while loop to continue on duplicates and an if to break on array end</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B62" authorId="0" shapeId="0" xr:uid="{7EB3A81C-A645-48D5-9C41-35C45B814EB6}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>downvoteit:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-Standard iterative binary search</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B63" authorId="0" shapeId="0" xr:uid="{B655BBA3-B037-4E4D-AA35-A7EC7D40AC70}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>downvoteit:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-Add all to set, traverse the array (for), if set.contains(n -1) is false then while set.contains(n+next) increament the next, Math.max(maxLen, curLen)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="205">
   <si>
     <t>#</t>
   </si>
@@ -784,13 +619,43 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/count-univalue-subtrees/</t>
+  </si>
+  <si>
+    <t>2016. Maximum Difference Between Increasing Elements</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-difference-between-increasing-elements/</t>
+  </si>
+  <si>
+    <t>122. Best Time to Buy and Sell Stock II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock-ii/</t>
+  </si>
+  <si>
+    <t>for i the array, add sum, if less than 0 reset to zero, Math.max(maxSum, curSum)</t>
+  </si>
+  <si>
+    <t>Add all to set, traverse the array (for), if set.contains(n -1) is false then while set.contains(n+next) increament the next, Math.max(maxLen, curLen)</t>
+  </si>
+  <si>
+    <t>Return if left + right == target else left++/right--</t>
+  </si>
+  <si>
+    <t>Modified binary search, return first if greater than last or smaller that first, else is an == statement, while loop to continue on duplicates and an if to break on array end</t>
+  </si>
+  <si>
+    <t>Standard iterative binary search</t>
+  </si>
+  <si>
+    <t>minLen = Integet.MAX_VALUE, for with winEnd, add n to minLen, while winSum &gt;= target Math.min(minLen, winEnd - winStart + 1) &amp;&amp; substract winStart from winSum &amp;&amp; increment winStart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -799,40 +664,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -866,23 +703,65 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="29">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1041,14 +920,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1327,22 +1198,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.28515625" customWidth="1"/>
     <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="173.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1369,252 +1240,279 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <f t="shared" ref="A2:A10" si="0">ROW()-1</f>
+      <c r="A2">
+        <f t="shared" ref="A2:A33" si="0">ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="B2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="4" t="s">
-        <v>146</v>
+      <c r="F3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="5"/>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="B5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="5"/>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="2"/>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="5"/>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
-        <v>37</v>
+      <c r="B9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s">
-        <v>37</v>
+      <c r="B10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>64</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>80</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>148</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>139</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" ref="A12:A43" si="1">ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>143</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>139</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>139</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>197</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>58</v>
+        <v>198</v>
       </c>
       <c r="D14" t="s">
-        <v>186</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
         <v>37</v>
@@ -1622,77 +1520,84 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>135</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F15" t="s">
         <v>37</v>
       </c>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F16" t="s">
         <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>159</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>158</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>3</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
@@ -1703,28 +1608,31 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s">
         <v>37</v>
+      </c>
+      <c r="G19" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -1745,152 +1653,149 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>139</v>
+        <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F21" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <f t="shared" si="1"/>
+      <c r="A22">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>146</v>
+      <c r="B22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" t="s">
+        <v>157</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <f t="shared" si="1"/>
+      <c r="A23">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>146</v>
+      <c r="B23" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="D24" t="s">
-        <v>139</v>
+        <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>144</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>139</v>
+        <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F25" t="s">
         <v>37</v>
       </c>
+      <c r="G25" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f t="shared" si="1"/>
+      <c r="A26" s="4">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" t="s">
-        <v>139</v>
-      </c>
-      <c r="E26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="B26" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>184</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>40</v>
+        <v>185</v>
       </c>
       <c r="D27" t="s">
-        <v>3</v>
+        <v>173</v>
       </c>
       <c r="E27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F27" t="s">
         <v>37</v>
@@ -1898,59 +1803,60 @@
     </row>
     <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>180</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>66</v>
+        <v>181</v>
       </c>
       <c r="D28" t="s">
-        <v>3</v>
+        <v>173</v>
       </c>
       <c r="E28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28"/>
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
+        <v>37</v>
+      </c>
       <c r="G28"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f t="shared" si="1"/>
+      <c r="A29" s="4">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" t="s">
-        <v>37</v>
-      </c>
-      <c r="G29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="D30" t="s">
-        <v>3</v>
+        <v>173</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1961,20 +1867,20 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>134</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>56</v>
+        <v>135</v>
       </c>
       <c r="D31" t="s">
-        <v>3</v>
+        <v>136</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F31" t="s">
         <v>37</v>
@@ -1982,140 +1888,143 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D32" t="s">
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F32" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>39</v>
+        <v>179</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="E33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A34:A59" si="1">ROW()-1</f>
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>118</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>119</v>
+        <v>51</v>
       </c>
       <c r="D34" t="s">
-        <v>166</v>
+        <v>17</v>
       </c>
       <c r="E34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>121</v>
+        <v>64</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="D35" t="s">
-        <v>166</v>
+        <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>151</v>
+        <v>6</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>152</v>
+        <v>52</v>
       </c>
       <c r="D36" t="s">
-        <v>166</v>
+        <v>17</v>
       </c>
       <c r="E36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F36" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>153</v>
+        <v>91</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="D37" t="s">
-        <v>157</v>
+        <v>33</v>
       </c>
       <c r="E37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="F37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>126</v>
+        <v>60</v>
       </c>
       <c r="D38" t="s">
-        <v>157</v>
+        <v>33</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
@@ -2123,20 +2032,23 @@
       <c r="F38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>124</v>
+        <v>26</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>125</v>
+        <v>46</v>
       </c>
       <c r="D39" t="s">
-        <v>157</v>
+        <v>33</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
@@ -2144,245 +2056,257 @@
       <c r="F39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>156</v>
+        <v>19</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>155</v>
+        <v>41</v>
       </c>
       <c r="D40" t="s">
-        <v>157</v>
+        <v>20</v>
       </c>
       <c r="E40" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="F40" t="s">
+        <v>37</v>
+      </c>
+      <c r="G40" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>130</v>
+        <v>49</v>
       </c>
       <c r="D41" t="s">
-        <v>173</v>
+        <v>18</v>
       </c>
       <c r="E41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>131</v>
+        <v>11</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>129</v>
+        <v>47</v>
       </c>
       <c r="D42" t="s">
-        <v>173</v>
+        <v>18</v>
       </c>
       <c r="E42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F42" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>132</v>
+        <v>10</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>133</v>
+        <v>48</v>
       </c>
       <c r="D43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" t="s">
         <v>173</v>
       </c>
-      <c r="E43" t="s">
-        <v>16</v>
-      </c>
-      <c r="F43" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
-        <f t="shared" ref="A44:A83" si="2">ROW()-1</f>
-        <v>43</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>184</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D45" t="s">
-        <v>173</v>
-      </c>
-      <c r="E45" t="s">
-        <v>15</v>
-      </c>
-      <c r="F45" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>180</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D46" t="s">
-        <v>173</v>
-      </c>
-      <c r="E46" t="s">
-        <v>15</v>
-      </c>
-      <c r="F46" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <f t="shared" si="2"/>
-        <v>46</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D48" t="s">
-        <v>173</v>
+        <v>3</v>
       </c>
       <c r="E48" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>192</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>94</v>
+        <v>191</v>
       </c>
       <c r="D49" t="s">
-        <v>173</v>
+        <v>20</v>
       </c>
       <c r="E49" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F49" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="D50" t="s">
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="E50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F50" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="D51" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E51" t="s">
         <v>16</v>
@@ -2391,19 +2315,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="D52" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E52" t="s">
         <v>16</v>
@@ -2412,251 +2336,234 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
       <c r="D53" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="E53" t="s">
         <v>15</v>
       </c>
-      <c r="G53" s="4"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>178</v>
+        <v>118</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>179</v>
+        <v>119</v>
       </c>
       <c r="D54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E54" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F54" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>140</v>
+        <v>29</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>141</v>
+        <v>39</v>
       </c>
       <c r="D55" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E55" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>140</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>51</v>
+        <v>141</v>
       </c>
       <c r="D56" t="s">
-        <v>17</v>
+        <v>139</v>
       </c>
       <c r="E56" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F56" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D57" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E57" t="s">
-        <v>15</v>
-      </c>
-      <c r="F57" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="B58" t="s">
-        <v>6</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D58" t="s">
-        <v>17</v>
-      </c>
-      <c r="E58" t="s">
-        <v>15</v>
-      </c>
-      <c r="F58" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="D59" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E59" t="s">
         <v>16</v>
       </c>
-      <c r="F59" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="2"/>
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>91</v>
+        <v>147</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>90</v>
+        <v>148</v>
       </c>
       <c r="D60" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E60" t="s">
-        <v>15</v>
-      </c>
-      <c r="F60" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
+        <f t="shared" ref="A61:A85" si="2">ROW()-1</f>
         <v>60</v>
       </c>
-      <c r="B61" t="s">
-        <v>32</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D61" t="s">
-        <v>33</v>
-      </c>
-      <c r="E61" t="s">
-        <v>15</v>
-      </c>
-      <c r="F61" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="B61" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
         <f t="shared" si="2"/>
         <v>61</v>
       </c>
-      <c r="B62" t="s">
-        <v>26</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D62" t="s">
-        <v>33</v>
-      </c>
-      <c r="E62" t="s">
-        <v>15</v>
-      </c>
-      <c r="F62" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="2"/>
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>12</v>
+        <v>193</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>43</v>
+        <v>194</v>
       </c>
       <c r="D63" t="s">
-        <v>18</v>
+        <v>173</v>
       </c>
       <c r="E63" t="s">
         <v>16</v>
       </c>
-      <c r="F63" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="D64" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E64" t="s">
-        <v>15</v>
-      </c>
-      <c r="F64" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2665,63 +2572,56 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>11</v>
+        <v>159</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>47</v>
+        <v>158</v>
       </c>
       <c r="D65" t="s">
-        <v>18</v>
+        <v>142</v>
       </c>
       <c r="E65" t="s">
-        <v>15</v>
-      </c>
-      <c r="F65" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
         <f t="shared" si="2"/>
         <v>65</v>
       </c>
-      <c r="B66" t="s">
-        <v>10</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D66" t="s">
-        <v>18</v>
-      </c>
-      <c r="E66" t="s">
-        <v>15</v>
-      </c>
-      <c r="F66" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67">
+      <c r="B66" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" s="2"/>
+      <c r="G66"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
         <f t="shared" si="2"/>
         <v>66</v>
       </c>
-      <c r="B67" t="s">
-        <v>9</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D67" t="s">
-        <v>18</v>
-      </c>
-      <c r="E67" t="s">
-        <v>15</v>
-      </c>
-      <c r="F67" t="s">
-        <v>37</v>
-      </c>
-      <c r="G67"/>
+      <c r="B67" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
@@ -2729,10 +2629,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>187</v>
+        <v>131</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>188</v>
+        <v>129</v>
       </c>
       <c r="D68" t="s">
         <v>73</v>
@@ -2742,25 +2642,23 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69">
+      <c r="A69" s="5">
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="B69" t="s">
-        <v>93</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D69" t="s">
-        <v>73</v>
-      </c>
-      <c r="E69" t="s">
-        <v>15</v>
-      </c>
-      <c r="F69" t="s">
-        <v>37</v>
-      </c>
+      <c r="B69" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
@@ -2768,16 +2666,16 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="D70" t="s">
         <v>73</v>
       </c>
       <c r="E70" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2786,16 +2684,16 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>104</v>
+        <v>154</v>
       </c>
       <c r="D71" t="s">
-        <v>73</v>
+        <v>157</v>
       </c>
       <c r="E71" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2804,13 +2702,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="D72" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="E72" t="s">
         <v>15</v>
@@ -2822,13 +2720,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>102</v>
+        <v>156</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>103</v>
+        <v>155</v>
       </c>
       <c r="D73" t="s">
-        <v>73</v>
+        <v>157</v>
       </c>
       <c r="E73" t="s">
         <v>15</v>
@@ -2840,34 +2738,39 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>89</v>
+        <v>150</v>
       </c>
       <c r="D74" t="s">
-        <v>73</v>
+        <v>168</v>
       </c>
       <c r="E74" t="s">
         <v>15</v>
       </c>
+      <c r="G74" s="4"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75">
+      <c r="A75" s="5">
         <f t="shared" si="2"/>
         <v>74</v>
       </c>
-      <c r="B75" t="s">
-        <v>106</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D75" t="s">
-        <v>73</v>
-      </c>
-      <c r="E75" t="s">
-        <v>15</v>
+      <c r="B75" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F75" s="5"/>
+      <c r="G75" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2876,10 +2779,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D76" t="s">
         <v>73</v>
@@ -2894,10 +2797,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="D77" t="s">
         <v>73</v>
@@ -2912,10 +2815,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="D78" t="s">
         <v>73</v>
@@ -2930,10 +2833,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D79" t="s">
         <v>73</v>
@@ -2948,10 +2851,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D80" t="s">
         <v>73</v>
@@ -2959,83 +2862,110 @@
       <c r="E80" t="s">
         <v>15</v>
       </c>
-      <c r="F80" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>190</v>
+        <v>106</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>189</v>
+        <v>107</v>
       </c>
       <c r="D81" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="E81" t="s">
         <v>15</v>
       </c>
-      <c r="F81" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>192</v>
+        <v>110</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>191</v>
+        <v>111</v>
       </c>
       <c r="D82" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="E82" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>193</v>
+        <v>87</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>194</v>
+        <v>86</v>
       </c>
       <c r="D83" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="E83" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <f t="shared" si="2"/>
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>115</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D84" t="s">
+        <v>73</v>
+      </c>
+      <c r="E84" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>187</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D85" t="s">
+        <v>73</v>
+      </c>
+      <c r="E85" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C84" s="1"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G78" xr:uid="{3809B7C5-5E24-49BB-A9E7-8AEF2B5426FA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G80">
-      <sortCondition sortBy="cellColor" ref="D1:D78" dxfId="23"/>
+  <autoFilter ref="A1:G85" xr:uid="{3809B7C5-5E24-49BB-A9E7-8AEF2B5426FA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G85">
+      <sortCondition ref="F1:F85"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="F55:F69 G20 G1 F72 F85:F1048576 F1:F53">
-    <cfRule type="containsText" dxfId="22" priority="39" operator="containsText" text="Solved">
+  <conditionalFormatting sqref="G20 G1 F71 F85:F1048576 F1:F53 F55 F57:F68">
+    <cfRule type="containsText" dxfId="28" priority="51" operator="containsText" text="Solved">
       <formula>NOT(ISERROR(SEARCH("Solved",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85:E1048576 E48:E51 E53 E1 E55:E69 E72">
-    <cfRule type="colorScale" priority="38">
+  <conditionalFormatting sqref="E85:E1048576 E48:E51 E53 E1 E55 E71 E57:E68">
+    <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0"/>
@@ -3047,22 +2977,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43">
-    <cfRule type="containsText" dxfId="21" priority="37" operator="containsText" text="Solved">
+    <cfRule type="containsText" dxfId="27" priority="49" operator="containsText" text="Solved">
       <formula>NOT(ISERROR(SEARCH("Solved",G43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="20" priority="36" operator="containsText" text="Solved">
+    <cfRule type="containsText" dxfId="26" priority="48" operator="containsText" text="Solved">
       <formula>NOT(ISERROR(SEARCH("Solved",G45)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F70">
-    <cfRule type="containsText" dxfId="19" priority="35" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F70)))</formula>
+  <conditionalFormatting sqref="F69">
+    <cfRule type="containsText" dxfId="25" priority="47" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F69)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E70">
-    <cfRule type="colorScale" priority="34">
+  <conditionalFormatting sqref="E69">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0"/>
@@ -3074,11 +3004,82 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54">
-    <cfRule type="containsText" dxfId="18" priority="33" operator="containsText" text="Solved">
+    <cfRule type="containsText" dxfId="24" priority="45" operator="containsText" text="Solved">
       <formula>NOT(ISERROR(SEARCH("Solved",F54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F70">
+    <cfRule type="containsText" dxfId="23" priority="43" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F70)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E70">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F72">
+    <cfRule type="containsText" dxfId="22" priority="38" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E72">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F73:F75">
+    <cfRule type="containsText" dxfId="21" priority="36" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F73)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E73:E75">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B86:B1048576 B1:B55 B57:B75">
+    <cfRule type="duplicateValues" dxfId="20" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F76">
+    <cfRule type="containsText" dxfId="19" priority="33" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F76)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E76">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -3090,13 +3091,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F71">
-    <cfRule type="containsText" dxfId="17" priority="31" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F71)))</formula>
+  <conditionalFormatting sqref="B76">
+    <cfRule type="duplicateValues" dxfId="18" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F77">
+    <cfRule type="containsText" dxfId="17" priority="30" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F77)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E71">
-    <cfRule type="colorScale" priority="30">
+  <conditionalFormatting sqref="E77">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0"/>
@@ -3107,13 +3111,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F73">
-    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F73)))</formula>
+  <conditionalFormatting sqref="B77">
+    <cfRule type="duplicateValues" dxfId="16" priority="28"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F78">
+    <cfRule type="containsText" dxfId="15" priority="27" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F78)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E73">
-    <cfRule type="colorScale" priority="25">
+  <conditionalFormatting sqref="E78">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0"/>
@@ -3124,12 +3131,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F74:F76">
-    <cfRule type="containsText" dxfId="15" priority="24" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F74)))</formula>
+  <conditionalFormatting sqref="B78">
+    <cfRule type="duplicateValues" dxfId="14" priority="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F79">
+    <cfRule type="containsText" dxfId="13" priority="24" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F79)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74:E76">
+  <conditionalFormatting sqref="E79">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -3141,15 +3151,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B85:B1048576 B1:B76">
-    <cfRule type="duplicateValues" dxfId="14" priority="22"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F77">
-    <cfRule type="containsText" dxfId="13" priority="21" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F77)))</formula>
+  <conditionalFormatting sqref="B79">
+    <cfRule type="duplicateValues" dxfId="12" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F80">
+    <cfRule type="containsText" dxfId="11" priority="21" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F80)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E77">
+  <conditionalFormatting sqref="E80">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -3161,15 +3171,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B77">
-    <cfRule type="duplicateValues" dxfId="12" priority="19"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F78">
-    <cfRule type="containsText" dxfId="11" priority="18" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F78)))</formula>
+  <conditionalFormatting sqref="B80">
+    <cfRule type="duplicateValues" dxfId="10" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F81">
+    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F81)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E78">
+  <conditionalFormatting sqref="E81">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -3181,15 +3191,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B78">
-    <cfRule type="duplicateValues" dxfId="10" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F79">
-    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F79)))</formula>
+  <conditionalFormatting sqref="B81">
+    <cfRule type="duplicateValues" dxfId="8" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F82">
+    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F82)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E79">
+  <conditionalFormatting sqref="E82">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -3201,35 +3211,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B79">
-    <cfRule type="duplicateValues" dxfId="8" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F80">
-    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F80)))</formula>
+  <conditionalFormatting sqref="B82">
+    <cfRule type="duplicateValues" dxfId="6" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F83">
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F83)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E80">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B80">
-    <cfRule type="duplicateValues" dxfId="6" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F81">
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F81)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E81">
+  <conditionalFormatting sqref="E83">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3241,15 +3231,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B81">
+  <conditionalFormatting sqref="B83">
     <cfRule type="duplicateValues" dxfId="4" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F82">
+  <conditionalFormatting sqref="F84">
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F82)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Solved",F84)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E82">
+  <conditionalFormatting sqref="E84">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3261,15 +3251,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B82">
+  <conditionalFormatting sqref="B84">
     <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F83:F84">
+  <conditionalFormatting sqref="F56">
     <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F83)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Solved",F56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E83:E84">
+  <conditionalFormatting sqref="E56">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3281,43 +3271,52 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B83:B84">
+  <conditionalFormatting sqref="B56">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C30" r:id="rId1" xr:uid="{AF582801-8C82-417A-BC90-754A4A4A273A}"/>
-    <hyperlink ref="C57" r:id="rId2" xr:uid="{93D7B805-0AAA-43DB-A5FB-8A47AFB4955F}"/>
-    <hyperlink ref="C9" r:id="rId3" xr:uid="{360E041F-B0DD-4BBB-99F0-FEC11C74DF66}"/>
-    <hyperlink ref="C10" r:id="rId4" xr:uid="{46F9E010-CBE8-4A2E-9C23-1ED4BB1B1F4E}"/>
-    <hyperlink ref="C16" r:id="rId5" xr:uid="{25A28752-23E4-47D8-A121-5D1EA00837E8}"/>
-    <hyperlink ref="C13" r:id="rId6" xr:uid="{3D1DAB51-3975-4C63-8024-DE42B1A10551}"/>
-    <hyperlink ref="C12" r:id="rId7" xr:uid="{A88D270B-DD4D-4B26-B375-EB9E13EFB360}"/>
-    <hyperlink ref="C19" r:id="rId8" xr:uid="{8212B78A-A644-47F5-98D0-3B1A37A7D45E}"/>
-    <hyperlink ref="C14" r:id="rId9" xr:uid="{7B89EAC2-F6B4-4EED-B8C9-86966B3540C8}"/>
-    <hyperlink ref="C29" r:id="rId10" xr:uid="{2CF0B45E-39BB-45F0-B562-6F6A109D4AE6}"/>
-    <hyperlink ref="C31" r:id="rId11" xr:uid="{F74243B0-9456-44C6-A8F8-7D4BC0097062}"/>
-    <hyperlink ref="C32" r:id="rId12" xr:uid="{9E0E15EC-C7D6-453F-BB20-B4DC44E847C0}"/>
-    <hyperlink ref="C27" r:id="rId13" xr:uid="{24945E02-001F-4EC2-B305-690B333CF5A7}"/>
-    <hyperlink ref="C28" r:id="rId14" xr:uid="{8EF49D9C-E60B-4173-BA06-3A5CB4948092}"/>
-    <hyperlink ref="C33" r:id="rId15" xr:uid="{EF98E54E-BA3E-4059-8787-256C26698DF2}"/>
-    <hyperlink ref="C56" r:id="rId16" xr:uid="{AFC88B2F-E281-44A4-B755-AEEEDC044D4E}"/>
-    <hyperlink ref="C58" r:id="rId17" xr:uid="{FCF2CE55-9407-4234-BD39-9931FA7929A1}"/>
-    <hyperlink ref="C7" r:id="rId18" xr:uid="{7170FF64-A78A-4745-A928-41A075FBEF23}"/>
-    <hyperlink ref="C61" r:id="rId19" xr:uid="{2D20E59F-FD49-4561-9516-026EFCBAC280}"/>
-    <hyperlink ref="C62" r:id="rId20" xr:uid="{E5A16AE2-EC0D-480F-92C4-628BBB8DF98B}"/>
-    <hyperlink ref="C64" r:id="rId21" xr:uid="{0F5CC868-171D-4ACE-AACF-92490F0A235F}"/>
-    <hyperlink ref="C8" r:id="rId22" xr:uid="{31C5E189-B075-4CA9-8FDB-D7FC91DE6008}"/>
-    <hyperlink ref="C65" r:id="rId23" xr:uid="{E7A6C803-C0F3-449E-8D52-3A4D7325CA42}"/>
-    <hyperlink ref="C66" r:id="rId24" xr:uid="{1CF48142-F48F-4E72-871F-8481378F69C0}"/>
-    <hyperlink ref="C63" r:id="rId25" xr:uid="{EB055FA2-9D2F-4517-AFA3-73B30C885722}"/>
-    <hyperlink ref="C23" r:id="rId26" xr:uid="{C6BE8D11-FA44-4BC5-873A-F1E866EC28B5}"/>
-    <hyperlink ref="C46" r:id="rId27" xr:uid="{BCF24D75-89DC-45DD-8C0B-B89E1D3DBFA4}"/>
-    <hyperlink ref="C67" r:id="rId28" xr:uid="{ECDFD730-14FE-4C5A-8BC7-5C597D35FD39}"/>
-    <hyperlink ref="C81" r:id="rId29" xr:uid="{F9644DAE-2375-4E11-B148-00AE9B96CA7F}"/>
-    <hyperlink ref="C78" r:id="rId30" xr:uid="{17F3C6CC-48F1-4E16-AD04-CA0F6EA0F43E}"/>
+    <hyperlink ref="C16" r:id="rId1" xr:uid="{AF582801-8C82-417A-BC90-754A4A4A273A}"/>
+    <hyperlink ref="C35" r:id="rId2" xr:uid="{93D7B805-0AAA-43DB-A5FB-8A47AFB4955F}"/>
+    <hyperlink ref="C25" r:id="rId3" xr:uid="{360E041F-B0DD-4BBB-99F0-FEC11C74DF66}"/>
+    <hyperlink ref="C21" r:id="rId4" xr:uid="{46F9E010-CBE8-4A2E-9C23-1ED4BB1B1F4E}"/>
+    <hyperlink ref="C40" r:id="rId5" xr:uid="{25A28752-23E4-47D8-A121-5D1EA00837E8}"/>
+    <hyperlink ref="C72" r:id="rId6" xr:uid="{3D1DAB51-3975-4C63-8024-DE42B1A10551}"/>
+    <hyperlink ref="C57" r:id="rId7" xr:uid="{A88D270B-DD4D-4B26-B375-EB9E13EFB360}"/>
+    <hyperlink ref="C7" r:id="rId8" xr:uid="{8212B78A-A644-47F5-98D0-3B1A37A7D45E}"/>
+    <hyperlink ref="C4" r:id="rId9" xr:uid="{7B89EAC2-F6B4-4EED-B8C9-86966B3540C8}"/>
+    <hyperlink ref="C15" r:id="rId10" xr:uid="{2CF0B45E-39BB-45F0-B562-6F6A109D4AE6}"/>
+    <hyperlink ref="C17" r:id="rId11" xr:uid="{F74243B0-9456-44C6-A8F8-7D4BC0097062}"/>
+    <hyperlink ref="C18" r:id="rId12" xr:uid="{9E0E15EC-C7D6-453F-BB20-B4DC44E847C0}"/>
+    <hyperlink ref="C32" r:id="rId13" xr:uid="{24945E02-001F-4EC2-B305-690B333CF5A7}"/>
+    <hyperlink ref="C64" r:id="rId14" xr:uid="{8EF49D9C-E60B-4173-BA06-3A5CB4948092}"/>
+    <hyperlink ref="C55" r:id="rId15" xr:uid="{EF98E54E-BA3E-4059-8787-256C26698DF2}"/>
+    <hyperlink ref="C34" r:id="rId16" xr:uid="{AFC88B2F-E281-44A4-B755-AEEEDC044D4E}"/>
+    <hyperlink ref="C36" r:id="rId17" xr:uid="{FCF2CE55-9407-4234-BD39-9931FA7929A1}"/>
+    <hyperlink ref="C66" r:id="rId18" xr:uid="{7170FF64-A78A-4745-A928-41A075FBEF23}"/>
+    <hyperlink ref="C38" r:id="rId19" xr:uid="{2D20E59F-FD49-4561-9516-026EFCBAC280}"/>
+    <hyperlink ref="C39" r:id="rId20" xr:uid="{E5A16AE2-EC0D-480F-92C4-628BBB8DF98B}"/>
+    <hyperlink ref="C41" r:id="rId21" xr:uid="{0F5CC868-171D-4ACE-AACF-92490F0A235F}"/>
+    <hyperlink ref="C67" r:id="rId22" xr:uid="{31C5E189-B075-4CA9-8FDB-D7FC91DE6008}"/>
+    <hyperlink ref="C42" r:id="rId23" xr:uid="{E7A6C803-C0F3-449E-8D52-3A4D7325CA42}"/>
+    <hyperlink ref="C43" r:id="rId24" xr:uid="{1CF48142-F48F-4E72-871F-8481378F69C0}"/>
+    <hyperlink ref="C19" r:id="rId25" xr:uid="{EB055FA2-9D2F-4517-AFA3-73B30C885722}"/>
+    <hyperlink ref="C10" r:id="rId26" xr:uid="{C6BE8D11-FA44-4BC5-873A-F1E866EC28B5}"/>
+    <hyperlink ref="C28" r:id="rId27" xr:uid="{BCF24D75-89DC-45DD-8C0B-B89E1D3DBFA4}"/>
+    <hyperlink ref="C44" r:id="rId28" xr:uid="{ECDFD730-14FE-4C5A-8BC7-5C597D35FD39}"/>
+    <hyperlink ref="C48" r:id="rId29" xr:uid="{F9644DAE-2375-4E11-B148-00AE9B96CA7F}"/>
+    <hyperlink ref="C46" r:id="rId30" xr:uid="{17F3C6CC-48F1-4E16-AD04-CA0F6EA0F43E}"/>
+    <hyperlink ref="C50" r:id="rId31" xr:uid="{48CB7216-5DE5-4684-8C98-214FEA373507}"/>
+    <hyperlink ref="C53" r:id="rId32" xr:uid="{FCC6530F-483D-4F94-A714-9E65F3331761}"/>
+    <hyperlink ref="C24" r:id="rId33" xr:uid="{F157EBA1-AA61-4D9A-9A0B-9B55DBB5A8D3}"/>
+    <hyperlink ref="C2" r:id="rId34" xr:uid="{1BF8D7CF-5169-4C51-8208-0334225B91B6}"/>
+    <hyperlink ref="C3" r:id="rId35" xr:uid="{F4285FE3-4FDE-4007-9456-FF7142723C52}"/>
+    <hyperlink ref="C5" r:id="rId36" xr:uid="{45D2EAC0-519A-4D4B-A91D-D076121D8E83}"/>
+    <hyperlink ref="C59" r:id="rId37" xr:uid="{A39EA5A2-4B4C-4792-88E5-3A106C4B97B4}"/>
+    <hyperlink ref="C68" r:id="rId38" xr:uid="{0060F7F0-2F01-4A54-A8A5-DA509EBDE87C}"/>
+    <hyperlink ref="C70" r:id="rId39" xr:uid="{A59214FE-37F1-4BCB-8FB8-D2425AE99834}"/>
+    <hyperlink ref="C75" r:id="rId40" xr:uid="{EE6108B9-B67A-4347-A1FF-7D6D16308B50}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
-  <legacyDrawing r:id="rId32"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DesignHashMap, DesignHashSet, PathSumII torture
</commit_message>
<xml_diff>
--- a/documents/Leetcode-problems.xlsx
+++ b/documents/Leetcode-problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\java-algorithms\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76ACDBE-59AE-4319-A341-BE6F774E3C11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E23FDD-878B-401C-A324-A1786D57E15C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Problems" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Problems!$A$1:$G$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Problems!$A$1:$G$84</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="211">
   <si>
     <t>#</t>
   </si>
@@ -661,6 +661,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/longest-univalue-path/</t>
+  </si>
+  <si>
+    <t>705. Design HashSet</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/design-hashset/</t>
   </si>
 </sst>
 </file>
@@ -731,7 +737,21 @@
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="37">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1255,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,16 +1361,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>171</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>58</v>
+        <v>172</v>
       </c>
       <c r="D4" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
         <v>37</v>
@@ -1362,13 +1382,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="D5" t="s">
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -1383,19 +1403,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
         <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1404,16 +1427,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
         <v>37</v>
@@ -1425,67 +1448,64 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>139</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>146</v>
+      <c r="B9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>146</v>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1494,18 +1514,18 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1515,16 +1535,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>144</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
         <v>37</v>
@@ -1536,19 +1556,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>139</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F13" t="s">
         <v>37</v>
+      </c>
+      <c r="G13" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1557,13 +1580,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>197</v>
+        <v>151</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>198</v>
+        <v>152</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>166</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
@@ -1578,21 +1601,20 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
+        <v>120</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>166</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F15" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1600,22 +1622,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>118</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>166</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F16" t="s">
         <v>37</v>
-      </c>
-      <c r="G16" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1624,16 +1643,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F17" t="s">
         <v>37</v>
@@ -1645,16 +1664,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>140</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>54</v>
+        <v>141</v>
       </c>
       <c r="D18" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s">
         <v>37</v>
@@ -1666,22 +1685,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>193</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>43</v>
+        <v>194</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>173</v>
       </c>
       <c r="E19" t="s">
         <v>16</v>
       </c>
       <c r="F19" t="s">
         <v>37</v>
-      </c>
-      <c r="G19" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1690,16 +1706,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>137</v>
+        <v>192</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>138</v>
+        <v>191</v>
       </c>
       <c r="D20" t="s">
-        <v>139</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F20" t="s">
         <v>37</v>
@@ -1711,16 +1727,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>186</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21" t="s">
         <v>37</v>
@@ -1732,13 +1748,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>127</v>
+        <v>85</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
@@ -1753,13 +1769,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>157</v>
+        <v>70</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>
@@ -1774,43 +1790,43 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>77</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>139</v>
       </c>
       <c r="E24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" t="s">
-        <v>37</v>
-      </c>
-      <c r="G25" t="s">
-        <v>201</v>
+      <c r="B25" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1819,19 +1835,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>37</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1840,18 +1859,18 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>184</v>
+        <v>80</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>185</v>
+        <v>81</v>
       </c>
       <c r="D27" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="E27" t="s">
         <v>15</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1861,13 +1880,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="D28" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
@@ -1878,23 +1897,23 @@
       <c r="G28"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="4" t="s">
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" t="s">
+        <v>139</v>
+      </c>
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1904,13 +1923,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="D30" t="s">
-        <v>173</v>
+        <v>3</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1918,6 +1937,7 @@
       <c r="F30" t="s">
         <v>37</v>
       </c>
+      <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1925,19 +1945,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>134</v>
+        <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="D31" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F31" t="s">
         <v>37</v>
+      </c>
+      <c r="G31" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1946,16 +1969,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D32" t="s">
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F32" t="s">
         <v>37</v>
@@ -1967,13 +1990,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>178</v>
+        <v>8</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>179</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>168</v>
+        <v>3</v>
       </c>
       <c r="E33" t="s">
         <v>15</v>
@@ -1984,17 +2007,17 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" ref="A34:A59" si="1">ROW()-1</f>
+        <f t="shared" ref="A34:A57" si="1">ROW()-1</f>
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>127</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>157</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
@@ -2009,13 +2032,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="D35" t="s">
-        <v>17</v>
+        <v>157</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
@@ -2025,23 +2048,23 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="4">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D36" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" t="s">
-        <v>15</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="B36" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2051,13 +2074,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>184</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>90</v>
+        <v>185</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>173</v>
       </c>
       <c r="E37" t="s">
         <v>15</v>
@@ -2072,13 +2095,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>60</v>
+        <v>181</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>173</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
@@ -2086,32 +2109,26 @@
       <c r="F38" t="s">
         <v>37</v>
       </c>
-      <c r="G38" t="s">
-        <v>202</v>
-      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="4">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B39" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" t="s">
-        <v>15</v>
-      </c>
-      <c r="F39" t="s">
-        <v>37</v>
-      </c>
-      <c r="G39" t="s">
-        <v>203</v>
+      <c r="B39" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2120,22 +2137,19 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>173</v>
       </c>
       <c r="E40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F40" t="s">
         <v>37</v>
-      </c>
-      <c r="G40" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2144,13 +2158,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>178</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>49</v>
+        <v>179</v>
       </c>
       <c r="D41" t="s">
-        <v>18</v>
+        <v>168</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
@@ -2165,13 +2179,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
@@ -2186,13 +2200,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="D43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
@@ -2207,13 +2221,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E44" t="s">
         <v>15</v>
@@ -2228,13 +2242,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
@@ -2249,19 +2263,22 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D46" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
       </c>
       <c r="F46" t="s">
         <v>37</v>
+      </c>
+      <c r="G46" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2270,19 +2287,22 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>97</v>
+        <v>26</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="D47" t="s">
-        <v>173</v>
+        <v>33</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
       </c>
       <c r="F47" t="s">
         <v>37</v>
+      </c>
+      <c r="G47" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2291,13 +2311,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>190</v>
+        <v>5</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>189</v>
+        <v>49</v>
       </c>
       <c r="D48" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E48" t="s">
         <v>15</v>
@@ -2312,16 +2332,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>192</v>
+        <v>11</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>191</v>
+        <v>47</v>
       </c>
       <c r="D49" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E49" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F49" t="s">
         <v>37</v>
@@ -2333,13 +2353,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>195</v>
+        <v>10</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>196</v>
+        <v>48</v>
       </c>
       <c r="D50" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E50" t="s">
         <v>15</v>
@@ -2354,16 +2374,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>151</v>
+        <v>9</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>152</v>
+        <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>166</v>
+        <v>18</v>
       </c>
       <c r="E51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F51" t="s">
         <v>37</v>
@@ -2375,16 +2395,16 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="D52" t="s">
-        <v>166</v>
+        <v>73</v>
       </c>
       <c r="E52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F52" t="s">
         <v>37</v>
@@ -2396,13 +2416,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>183</v>
+        <v>72</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>182</v>
+        <v>71</v>
       </c>
       <c r="D53" t="s">
-        <v>173</v>
+        <v>20</v>
       </c>
       <c r="E53" t="s">
         <v>15</v>
@@ -2417,16 +2437,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="D54" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F54" t="s">
         <v>37</v>
@@ -2438,16 +2458,16 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>29</v>
+        <v>190</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>39</v>
+        <v>189</v>
       </c>
       <c r="D55" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F55" t="s">
         <v>37</v>
@@ -2459,16 +2479,16 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>140</v>
+        <v>195</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>141</v>
+        <v>196</v>
       </c>
       <c r="D56" t="s">
-        <v>139</v>
+        <v>20</v>
       </c>
       <c r="E56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F56" t="s">
         <v>37</v>
@@ -2480,123 +2500,135 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>62</v>
+        <v>183</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>63</v>
+        <v>182</v>
       </c>
       <c r="D57" t="s">
-        <v>31</v>
+        <v>173</v>
       </c>
       <c r="E57" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F57" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="5">
-        <f t="shared" si="1"/>
-        <v>57</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F58" s="5"/>
+      <c r="A58">
+        <v>86</v>
+      </c>
+      <c r="B58" t="s">
+        <v>206</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D58" t="s">
+        <v>173</v>
+      </c>
+      <c r="E58" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="D59" t="s">
-        <v>73</v>
+        <v>157</v>
       </c>
       <c r="E59" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F59" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>64</v>
+        <f>ROW()-1</f>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>147</v>
+        <v>209</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>148</v>
+        <v>210</v>
       </c>
       <c r="D60" t="s">
+        <v>157</v>
+      </c>
+      <c r="E60" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f>ROW()-1</f>
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61" t="s">
         <v>31</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E61" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
-        <f t="shared" ref="A61:A88" si="2">ROW()-1</f>
-        <v>60</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>61</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F62" s="5"/>
+      <c r="F62" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>193</v>
+        <v>132</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>194</v>
+        <v>133</v>
       </c>
       <c r="D63" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="E63" t="s">
         <v>16</v>
@@ -2604,78 +2636,77 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="2"/>
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>147</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>66</v>
+        <v>148</v>
       </c>
       <c r="D64" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E64" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <f t="shared" si="2"/>
+    <row r="65" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <f t="shared" ref="A65:A88" si="2">ROW()-1</f>
         <v>64</v>
       </c>
-      <c r="B65" t="s">
-        <v>159</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D65" t="s">
-        <v>142</v>
-      </c>
-      <c r="E65" t="s">
+      <c r="B65" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
+      <c r="F65" s="5"/>
+      <c r="G65"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
         <f t="shared" si="2"/>
         <v>65</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E66" s="2" t="s">
+      <c r="B66" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F66" s="2"/>
-      <c r="G66"/>
+      <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="5">
+      <c r="A67">
         <f t="shared" si="2"/>
         <v>66</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F67" s="5"/>
+      <c r="B67" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D67" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
@@ -2683,36 +2714,36 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="D68" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="E68" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="5">
+      <c r="A69" s="2">
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="E69" s="5" t="s">
+      <c r="B69" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F69" s="5"/>
+      <c r="F69" s="2"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
@@ -2720,10 +2751,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D70" t="s">
         <v>73</v>
@@ -2733,22 +2764,23 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71">
+      <c r="A71" s="5">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="B71" t="s">
-        <v>153</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D71" t="s">
-        <v>157</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="B71" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="F71" s="5"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
@@ -2756,16 +2788,16 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>35</v>
+        <v>128</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>61</v>
+        <v>130</v>
       </c>
       <c r="D72" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="E72" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2774,57 +2806,56 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D73" t="s">
         <v>157</v>
       </c>
       <c r="E73" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74">
+      <c r="A74" s="5">
         <f t="shared" si="2"/>
         <v>73</v>
       </c>
-      <c r="B74" t="s">
-        <v>149</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D74" t="s">
-        <v>168</v>
-      </c>
-      <c r="E74" t="s">
-        <v>15</v>
-      </c>
-      <c r="G74" s="4"/>
+      <c r="B74" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F74" s="5"/>
+      <c r="G74" s="4" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="5">
+      <c r="A75">
         <f t="shared" si="2"/>
         <v>74</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E75" s="5" t="s">
+      <c r="B75" t="s">
+        <v>187</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D75" t="s">
+        <v>73</v>
+      </c>
+      <c r="E75" t="s">
         <v>16</v>
-      </c>
-      <c r="F75" s="5"/>
-      <c r="G75" s="4" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2833,35 +2864,39 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>113</v>
+        <v>207</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>112</v>
+        <v>208</v>
       </c>
       <c r="D76" t="s">
-        <v>73</v>
+        <v>173</v>
       </c>
       <c r="E76" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="F76" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77">
+      <c r="A77" s="5">
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
-      <c r="B77" t="s">
-        <v>105</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D77" t="s">
-        <v>73</v>
-      </c>
-      <c r="E77" t="s">
-        <v>15</v>
-      </c>
+      <c r="B77" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
@@ -2869,13 +2904,13 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="D78" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="E78" t="s">
         <v>15</v>
@@ -2887,17 +2922,18 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>103</v>
+        <v>150</v>
       </c>
       <c r="D79" t="s">
-        <v>73</v>
+        <v>168</v>
       </c>
       <c r="E79" t="s">
         <v>15</v>
       </c>
+      <c r="G79" s="4"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
@@ -2905,10 +2941,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="D80" t="s">
         <v>73</v>
@@ -2917,16 +2953,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D81" t="s">
         <v>73</v>
@@ -2935,16 +2971,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D82" t="s">
         <v>73</v>
@@ -2953,16 +2989,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="D83" t="s">
         <v>73</v>
@@ -2971,16 +3007,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="2"/>
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="D84" t="s">
         <v>73</v>
@@ -2989,96 +3025,91 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>187</v>
+        <v>106</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>188</v>
+        <v>107</v>
       </c>
       <c r="D85" t="s">
         <v>73</v>
       </c>
       <c r="E85" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>193</v>
+        <v>110</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>194</v>
+        <v>111</v>
       </c>
       <c r="D86" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="E86" t="s">
-        <v>16</v>
-      </c>
-      <c r="F86" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
+        <f t="shared" si="2"/>
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>206</v>
+        <v>87</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>205</v>
+        <v>86</v>
       </c>
       <c r="D87" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
       </c>
-      <c r="F87" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="2"/>
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>207</v>
+        <v>115</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>208</v>
+        <v>114</v>
       </c>
       <c r="D88" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="E88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G85" xr:uid="{3809B7C5-5E24-49BB-A9E7-8AEF2B5426FA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G85">
-      <sortCondition ref="F1:F85"/>
+  <autoFilter ref="A1:G84" xr:uid="{3809B7C5-5E24-49BB-A9E7-8AEF2B5426FA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G88">
+      <sortCondition descending="1" ref="F1:F84"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="G20 G1 F71 F85 F1:F53 F55 F57:F68 F89:F1048576">
-    <cfRule type="containsText" dxfId="34" priority="60" operator="containsText" text="Solved">
+  <conditionalFormatting sqref="G20 G1 F70 F84 F1:F53 F55 F89:F1048576 F57:F67">
+    <cfRule type="containsText" dxfId="36" priority="63" operator="containsText" text="Solved">
       <formula>NOT(ISERROR(SEARCH("Solved",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48:E51 E85 E53 E1 E55 E71 E57:E68 E89:E1048576">
-    <cfRule type="colorScale" priority="59">
+  <conditionalFormatting sqref="E48:E51 E84 E53 E1 E55 E70 E57:E67 E89:E1048576">
+    <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0"/>
@@ -3090,22 +3121,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43">
-    <cfRule type="containsText" dxfId="33" priority="58" operator="containsText" text="Solved">
+    <cfRule type="containsText" dxfId="35" priority="61" operator="containsText" text="Solved">
       <formula>NOT(ISERROR(SEARCH("Solved",G43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="32" priority="57" operator="containsText" text="Solved">
+    <cfRule type="containsText" dxfId="34" priority="60" operator="containsText" text="Solved">
       <formula>NOT(ISERROR(SEARCH("Solved",G45)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F69">
-    <cfRule type="containsText" dxfId="31" priority="56" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F69)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
-    <cfRule type="colorScale" priority="55">
+  <conditionalFormatting sqref="F68">
+    <cfRule type="containsText" dxfId="33" priority="59" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F68)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E68">
+    <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0"/>
@@ -3117,12 +3148,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54">
-    <cfRule type="containsText" dxfId="30" priority="54" operator="containsText" text="Solved">
+    <cfRule type="containsText" dxfId="32" priority="57" operator="containsText" text="Solved">
       <formula>NOT(ISERROR(SEARCH("Solved",F54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54">
-    <cfRule type="colorScale" priority="53">
+    <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0"/>
@@ -3133,13 +3164,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F70">
-    <cfRule type="containsText" dxfId="29" priority="52" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F70)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E70">
-    <cfRule type="colorScale" priority="51">
+  <conditionalFormatting sqref="F69">
+    <cfRule type="containsText" dxfId="31" priority="55" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69">
+    <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0"/>
@@ -3150,13 +3181,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F72">
-    <cfRule type="containsText" dxfId="28" priority="47" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F72)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E72">
-    <cfRule type="colorScale" priority="46">
+  <conditionalFormatting sqref="F71">
+    <cfRule type="containsText" dxfId="30" priority="50" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F71)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E71">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0"/>
@@ -3167,12 +3198,32 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F73:F75">
+  <conditionalFormatting sqref="F72:F74">
+    <cfRule type="containsText" dxfId="29" priority="48" operator="containsText" text="Solved">
+      <formula>NOT(ISERROR(SEARCH("Solved",F72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E72:E74">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B89:B1048576 B1:B55 B57:B74">
+    <cfRule type="duplicateValues" dxfId="28" priority="46"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F75">
     <cfRule type="containsText" dxfId="27" priority="45" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F73)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E73:E75">
+      <formula>NOT(ISERROR(SEARCH("Solved",F75)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E75">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -3184,7 +3235,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B89:B1048576 B1:B55 B57:B75">
+  <conditionalFormatting sqref="B75">
     <cfRule type="duplicateValues" dxfId="26" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F76">
@@ -3308,12 +3359,12 @@
     <cfRule type="duplicateValues" dxfId="14" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F82">
-    <cfRule type="containsText" dxfId="13" priority="24" operator="containsText" text="Solved">
+    <cfRule type="containsText" dxfId="13" priority="21" operator="containsText" text="Solved">
       <formula>NOT(ISERROR(SEARCH("Solved",F82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E82">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="0"/>
@@ -3325,7 +3376,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82">
-    <cfRule type="duplicateValues" dxfId="12" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F83">
     <cfRule type="containsText" dxfId="11" priority="18" operator="containsText" text="Solved">
@@ -3347,12 +3398,12 @@
   <conditionalFormatting sqref="B83">
     <cfRule type="duplicateValues" dxfId="10" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F84">
+  <conditionalFormatting sqref="F56">
     <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F84)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E84">
+      <formula>NOT(ISERROR(SEARCH("Solved",F56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E56">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -3364,15 +3415,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B84">
+  <conditionalFormatting sqref="B56">
     <cfRule type="duplicateValues" dxfId="8" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F56">
+  <conditionalFormatting sqref="F85">
     <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="Solved">
-      <formula>NOT(ISERROR(SEARCH("Solved",F56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E56">
+      <formula>NOT(ISERROR(SEARCH("Solved",F85)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E85">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -3384,7 +3435,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B56">
+  <conditionalFormatting sqref="B85">
     <cfRule type="duplicateValues" dxfId="6" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F86">
@@ -3448,46 +3499,46 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C16" r:id="rId1" xr:uid="{AF582801-8C82-417A-BC90-754A4A4A273A}"/>
-    <hyperlink ref="C35" r:id="rId2" xr:uid="{93D7B805-0AAA-43DB-A5FB-8A47AFB4955F}"/>
-    <hyperlink ref="C25" r:id="rId3" xr:uid="{360E041F-B0DD-4BBB-99F0-FEC11C74DF66}"/>
-    <hyperlink ref="C21" r:id="rId4" xr:uid="{46F9E010-CBE8-4A2E-9C23-1ED4BB1B1F4E}"/>
-    <hyperlink ref="C40" r:id="rId5" xr:uid="{25A28752-23E4-47D8-A121-5D1EA00837E8}"/>
-    <hyperlink ref="C72" r:id="rId6" xr:uid="{3D1DAB51-3975-4C63-8024-DE42B1A10551}"/>
-    <hyperlink ref="C57" r:id="rId7" xr:uid="{A88D270B-DD4D-4B26-B375-EB9E13EFB360}"/>
-    <hyperlink ref="C7" r:id="rId8" xr:uid="{8212B78A-A644-47F5-98D0-3B1A37A7D45E}"/>
-    <hyperlink ref="C4" r:id="rId9" xr:uid="{7B89EAC2-F6B4-4EED-B8C9-86966B3540C8}"/>
-    <hyperlink ref="C15" r:id="rId10" xr:uid="{2CF0B45E-39BB-45F0-B562-6F6A109D4AE6}"/>
-    <hyperlink ref="C17" r:id="rId11" xr:uid="{F74243B0-9456-44C6-A8F8-7D4BC0097062}"/>
-    <hyperlink ref="C18" r:id="rId12" xr:uid="{9E0E15EC-C7D6-453F-BB20-B4DC44E847C0}"/>
-    <hyperlink ref="C32" r:id="rId13" xr:uid="{24945E02-001F-4EC2-B305-690B333CF5A7}"/>
-    <hyperlink ref="C64" r:id="rId14" xr:uid="{8EF49D9C-E60B-4173-BA06-3A5CB4948092}"/>
-    <hyperlink ref="C55" r:id="rId15" xr:uid="{EF98E54E-BA3E-4059-8787-256C26698DF2}"/>
-    <hyperlink ref="C34" r:id="rId16" xr:uid="{AFC88B2F-E281-44A4-B755-AEEEDC044D4E}"/>
-    <hyperlink ref="C36" r:id="rId17" xr:uid="{FCF2CE55-9407-4234-BD39-9931FA7929A1}"/>
-    <hyperlink ref="C66" r:id="rId18" xr:uid="{7170FF64-A78A-4745-A928-41A075FBEF23}"/>
-    <hyperlink ref="C38" r:id="rId19" xr:uid="{2D20E59F-FD49-4561-9516-026EFCBAC280}"/>
-    <hyperlink ref="C39" r:id="rId20" xr:uid="{E5A16AE2-EC0D-480F-92C4-628BBB8DF98B}"/>
-    <hyperlink ref="C41" r:id="rId21" xr:uid="{0F5CC868-171D-4ACE-AACF-92490F0A235F}"/>
-    <hyperlink ref="C67" r:id="rId22" xr:uid="{31C5E189-B075-4CA9-8FDB-D7FC91DE6008}"/>
-    <hyperlink ref="C42" r:id="rId23" xr:uid="{E7A6C803-C0F3-449E-8D52-3A4D7325CA42}"/>
-    <hyperlink ref="C43" r:id="rId24" xr:uid="{1CF48142-F48F-4E72-871F-8481378F69C0}"/>
-    <hyperlink ref="C19" r:id="rId25" xr:uid="{EB055FA2-9D2F-4517-AFA3-73B30C885722}"/>
-    <hyperlink ref="C10" r:id="rId26" xr:uid="{C6BE8D11-FA44-4BC5-873A-F1E866EC28B5}"/>
-    <hyperlink ref="C28" r:id="rId27" xr:uid="{BCF24D75-89DC-45DD-8C0B-B89E1D3DBFA4}"/>
-    <hyperlink ref="C44" r:id="rId28" xr:uid="{ECDFD730-14FE-4C5A-8BC7-5C597D35FD39}"/>
-    <hyperlink ref="C48" r:id="rId29" xr:uid="{F9644DAE-2375-4E11-B148-00AE9B96CA7F}"/>
-    <hyperlink ref="C46" r:id="rId30" xr:uid="{17F3C6CC-48F1-4E16-AD04-CA0F6EA0F43E}"/>
-    <hyperlink ref="C50" r:id="rId31" xr:uid="{48CB7216-5DE5-4684-8C98-214FEA373507}"/>
-    <hyperlink ref="C53" r:id="rId32" xr:uid="{FCC6530F-483D-4F94-A714-9E65F3331761}"/>
-    <hyperlink ref="C24" r:id="rId33" xr:uid="{F157EBA1-AA61-4D9A-9A0B-9B55DBB5A8D3}"/>
+    <hyperlink ref="C31" r:id="rId1" xr:uid="{AF582801-8C82-417A-BC90-754A4A4A273A}"/>
+    <hyperlink ref="C43" r:id="rId2" xr:uid="{93D7B805-0AAA-43DB-A5FB-8A47AFB4955F}"/>
+    <hyperlink ref="C10" r:id="rId3" xr:uid="{360E041F-B0DD-4BBB-99F0-FEC11C74DF66}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{46F9E010-CBE8-4A2E-9C23-1ED4BB1B1F4E}"/>
+    <hyperlink ref="C13" r:id="rId5" xr:uid="{25A28752-23E4-47D8-A121-5D1EA00837E8}"/>
+    <hyperlink ref="C78" r:id="rId6" xr:uid="{3D1DAB51-3975-4C63-8024-DE42B1A10551}"/>
+    <hyperlink ref="C61" r:id="rId7" xr:uid="{A88D270B-DD4D-4B26-B375-EB9E13EFB360}"/>
+    <hyperlink ref="C23" r:id="rId8" xr:uid="{8212B78A-A644-47F5-98D0-3B1A37A7D45E}"/>
+    <hyperlink ref="C21" r:id="rId9" xr:uid="{7B89EAC2-F6B4-4EED-B8C9-86966B3540C8}"/>
+    <hyperlink ref="C30" r:id="rId10" xr:uid="{2CF0B45E-39BB-45F0-B562-6F6A109D4AE6}"/>
+    <hyperlink ref="C32" r:id="rId11" xr:uid="{F74243B0-9456-44C6-A8F8-7D4BC0097062}"/>
+    <hyperlink ref="C33" r:id="rId12" xr:uid="{9E0E15EC-C7D6-453F-BB20-B4DC44E847C0}"/>
+    <hyperlink ref="C12" r:id="rId13" xr:uid="{24945E02-001F-4EC2-B305-690B333CF5A7}"/>
+    <hyperlink ref="C67" r:id="rId14" xr:uid="{8EF49D9C-E60B-4173-BA06-3A5CB4948092}"/>
+    <hyperlink ref="C17" r:id="rId15" xr:uid="{EF98E54E-BA3E-4059-8787-256C26698DF2}"/>
+    <hyperlink ref="C42" r:id="rId16" xr:uid="{AFC88B2F-E281-44A4-B755-AEEEDC044D4E}"/>
+    <hyperlink ref="C44" r:id="rId17" xr:uid="{FCF2CE55-9407-4234-BD39-9931FA7929A1}"/>
+    <hyperlink ref="C69" r:id="rId18" xr:uid="{7170FF64-A78A-4745-A928-41A075FBEF23}"/>
+    <hyperlink ref="C46" r:id="rId19" xr:uid="{2D20E59F-FD49-4561-9516-026EFCBAC280}"/>
+    <hyperlink ref="C47" r:id="rId20" xr:uid="{E5A16AE2-EC0D-480F-92C4-628BBB8DF98B}"/>
+    <hyperlink ref="C48" r:id="rId21" xr:uid="{0F5CC868-171D-4ACE-AACF-92490F0A235F}"/>
+    <hyperlink ref="C77" r:id="rId22" xr:uid="{31C5E189-B075-4CA9-8FDB-D7FC91DE6008}"/>
+    <hyperlink ref="C49" r:id="rId23" xr:uid="{E7A6C803-C0F3-449E-8D52-3A4D7325CA42}"/>
+    <hyperlink ref="C50" r:id="rId24" xr:uid="{1CF48142-F48F-4E72-871F-8481378F69C0}"/>
+    <hyperlink ref="C6" r:id="rId25" xr:uid="{EB055FA2-9D2F-4517-AFA3-73B30C885722}"/>
+    <hyperlink ref="C26" r:id="rId26" xr:uid="{C6BE8D11-FA44-4BC5-873A-F1E866EC28B5}"/>
+    <hyperlink ref="C38" r:id="rId27" xr:uid="{BCF24D75-89DC-45DD-8C0B-B89E1D3DBFA4}"/>
+    <hyperlink ref="C51" r:id="rId28" xr:uid="{ECDFD730-14FE-4C5A-8BC7-5C597D35FD39}"/>
+    <hyperlink ref="C55" r:id="rId29" xr:uid="{F9644DAE-2375-4E11-B148-00AE9B96CA7F}"/>
+    <hyperlink ref="C53" r:id="rId30" xr:uid="{17F3C6CC-48F1-4E16-AD04-CA0F6EA0F43E}"/>
+    <hyperlink ref="C56" r:id="rId31" xr:uid="{48CB7216-5DE5-4684-8C98-214FEA373507}"/>
+    <hyperlink ref="C57" r:id="rId32" xr:uid="{FCC6530F-483D-4F94-A714-9E65F3331761}"/>
+    <hyperlink ref="C9" r:id="rId33" xr:uid="{F157EBA1-AA61-4D9A-9A0B-9B55DBB5A8D3}"/>
     <hyperlink ref="C2" r:id="rId34" xr:uid="{1BF8D7CF-5169-4C51-8208-0334225B91B6}"/>
     <hyperlink ref="C3" r:id="rId35" xr:uid="{F4285FE3-4FDE-4007-9456-FF7142723C52}"/>
-    <hyperlink ref="C5" r:id="rId36" xr:uid="{45D2EAC0-519A-4D4B-A91D-D076121D8E83}"/>
-    <hyperlink ref="C59" r:id="rId37" xr:uid="{A39EA5A2-4B4C-4792-88E5-3A106C4B97B4}"/>
-    <hyperlink ref="C68" r:id="rId38" xr:uid="{0060F7F0-2F01-4A54-A8A5-DA509EBDE87C}"/>
-    <hyperlink ref="C70" r:id="rId39" xr:uid="{A59214FE-37F1-4BCB-8FB8-D2425AE99834}"/>
-    <hyperlink ref="C75" r:id="rId40" xr:uid="{EE6108B9-B67A-4347-A1FF-7D6D16308B50}"/>
+    <hyperlink ref="C4" r:id="rId36" xr:uid="{45D2EAC0-519A-4D4B-A91D-D076121D8E83}"/>
+    <hyperlink ref="C63" r:id="rId37" xr:uid="{A39EA5A2-4B4C-4792-88E5-3A106C4B97B4}"/>
+    <hyperlink ref="C70" r:id="rId38" xr:uid="{0060F7F0-2F01-4A54-A8A5-DA509EBDE87C}"/>
+    <hyperlink ref="C72" r:id="rId39" xr:uid="{A59214FE-37F1-4BCB-8FB8-D2425AE99834}"/>
+    <hyperlink ref="C74" r:id="rId40" xr:uid="{EE6108B9-B67A-4347-A1FF-7D6D16308B50}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>

</xml_diff>

<commit_message>
DiameterOfBinaryTree, TwoSum more solutions
</commit_message>
<xml_diff>
--- a/documents/Leetcode-problems.xlsx
+++ b/documents/Leetcode-problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\java-algorithms\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E23FDD-878B-401C-A324-A1786D57E15C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88A06AD-E020-41DB-8BB9-DE9DCD949151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="211">
   <si>
     <t>#</t>
   </si>
@@ -1276,7 +1276,7 @@
   <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2953,7 +2953,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="2"/>
         <v>80</v>
@@ -2971,7 +2971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="2"/>
         <v>81</v>
@@ -2989,7 +2989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="2"/>
         <v>82</v>
@@ -3001,13 +3001,16 @@
         <v>103</v>
       </c>
       <c r="D83" t="s">
-        <v>73</v>
+        <v>173</v>
       </c>
       <c r="E83" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F83" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="2"/>
         <v>83</v>
@@ -3025,7 +3028,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="2"/>
         <v>84</v>
@@ -3043,7 +3046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="2"/>
         <v>85</v>
@@ -3061,7 +3064,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="2"/>
         <v>86</v>
@@ -3079,7 +3082,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="2"/>
         <v>87</v>

</xml_diff>

<commit_message>
Tree problem test case refactoring
</commit_message>
<xml_diff>
--- a/documents/Leetcode-problems.xlsx
+++ b/documents/Leetcode-problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\java-algorithms\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88A06AD-E020-41DB-8BB9-DE9DCD949151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F53783-36B2-4B2A-A52A-7C3F0DFAC9EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1275,8 +1275,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1316,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f t="shared" ref="A2:A33" si="0">ROW()-1</f>
+        <f>ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1336,7 +1337,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1357,7 +1358,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1378,7 +1379,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -1399,7 +1400,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -1423,7 +1424,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -1444,7 +1445,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -1465,7 +1466,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -1486,7 +1487,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -1510,7 +1511,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -1531,7 +1532,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -1552,7 +1553,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -1576,7 +1577,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -1597,7 +1598,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -1618,7 +1619,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>15</v>
       </c>
       <c r="B16" t="s">
@@ -1639,7 +1640,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -1660,7 +1661,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -1681,7 +1682,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>18</v>
       </c>
       <c r="B19" t="s">
@@ -1702,7 +1703,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -1723,7 +1724,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -1744,7 +1745,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -1765,7 +1766,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -1786,7 +1787,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>23</v>
       </c>
       <c r="B24" t="s">
@@ -1807,7 +1808,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -1831,7 +1832,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1855,7 +1856,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>26</v>
       </c>
       <c r="B27" t="s">
@@ -1876,7 +1877,7 @@
     </row>
     <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>27</v>
       </c>
       <c r="B28" t="s">
@@ -1898,7 +1899,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>28</v>
       </c>
       <c r="B29" t="s">
@@ -1919,7 +1920,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>29</v>
       </c>
       <c r="B30" t="s">
@@ -1941,7 +1942,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>30</v>
       </c>
       <c r="B31" t="s">
@@ -1965,7 +1966,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>31</v>
       </c>
       <c r="B32" t="s">
@@ -1986,7 +1987,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>32</v>
       </c>
       <c r="B33" t="s">
@@ -2007,7 +2008,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" ref="A34:A57" si="1">ROW()-1</f>
+        <f>ROW()-1</f>
         <v>33</v>
       </c>
       <c r="B34" t="s">
@@ -2028,7 +2029,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>34</v>
       </c>
       <c r="B35" t="s">
@@ -2049,7 +2050,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -2070,7 +2071,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>36</v>
       </c>
       <c r="B37" t="s">
@@ -2091,7 +2092,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>37</v>
       </c>
       <c r="B38" t="s">
@@ -2112,7 +2113,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -2133,7 +2134,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>39</v>
       </c>
       <c r="B40" t="s">
@@ -2154,7 +2155,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>40</v>
       </c>
       <c r="B41" t="s">
@@ -2175,7 +2176,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>41</v>
       </c>
       <c r="B42" t="s">
@@ -2196,7 +2197,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>42</v>
       </c>
       <c r="B43" t="s">
@@ -2217,7 +2218,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>43</v>
       </c>
       <c r="B44" t="s">
@@ -2238,7 +2239,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>44</v>
       </c>
       <c r="B45" t="s">
@@ -2259,7 +2260,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>45</v>
       </c>
       <c r="B46" t="s">
@@ -2283,7 +2284,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>46</v>
       </c>
       <c r="B47" t="s">
@@ -2307,7 +2308,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>47</v>
       </c>
       <c r="B48" t="s">
@@ -2328,7 +2329,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>48</v>
       </c>
       <c r="B49" t="s">
@@ -2349,7 +2350,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>49</v>
       </c>
       <c r="B50" t="s">
@@ -2370,7 +2371,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>50</v>
       </c>
       <c r="B51" t="s">
@@ -2391,7 +2392,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>51</v>
       </c>
       <c r="B52" t="s">
@@ -2412,7 +2413,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>52</v>
       </c>
       <c r="B53" t="s">
@@ -2433,7 +2434,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>53</v>
       </c>
       <c r="B54" t="s">
@@ -2454,7 +2455,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>54</v>
       </c>
       <c r="B55" t="s">
@@ -2475,7 +2476,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>55</v>
       </c>
       <c r="B56" t="s">
@@ -2496,7 +2497,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>56</v>
       </c>
       <c r="B57" t="s">
@@ -2578,41 +2579,44 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="A61" s="5">
         <f>ROW()-1</f>
         <v>60</v>
       </c>
-      <c r="B61" t="s">
-        <v>62</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D61" t="s">
-        <v>31</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="B61" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="F61" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="5">
+      <c r="A62">
         <f>ROW()-1</f>
         <v>61</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E62" s="5" t="s">
+      <c r="B62" t="s">
+        <v>207</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D62" t="s">
+        <v>173</v>
+      </c>
+      <c r="E62" t="s">
         <v>16</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F62" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2622,27 +2626,31 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="D63" t="s">
-        <v>73</v>
+        <v>173</v>
       </c>
       <c r="E63" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F63" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>64</v>
+        <f>ROW()-1</f>
+        <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>147</v>
+        <v>62</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>148</v>
+        <v>63</v>
       </c>
       <c r="D64" t="s">
         <v>31</v>
@@ -2652,146 +2660,145 @@
       </c>
     </row>
     <row r="65" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
-        <f t="shared" ref="A65:A88" si="2">ROW()-1</f>
+      <c r="A65">
+        <f>ROW()-1</f>
         <v>64</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D65" t="s">
+        <v>73</v>
+      </c>
+      <c r="E65" t="s">
+        <v>16</v>
+      </c>
+      <c r="F65"/>
+      <c r="G65"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>147</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D66" t="s">
+        <v>31</v>
+      </c>
+      <c r="E66" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
+        <f>ROW()-1</f>
+        <v>66</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C67" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D67" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="E65" s="5" t="s">
+      <c r="E67" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F65" s="5"/>
-      <c r="G65"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="5">
-        <f t="shared" si="2"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="5">
+        <f>ROW()-1</f>
+        <v>67</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f>ROW()-1</f>
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="E66" s="5" t="s">
+      <c r="C69" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D69" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" t="s">
         <v>16</v>
       </c>
-      <c r="F66" s="5"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <f t="shared" si="2"/>
-        <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>65</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D67" t="s">
-        <v>3</v>
-      </c>
-      <c r="E67" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <f t="shared" si="2"/>
-        <v>67</v>
-      </c>
-      <c r="B68" t="s">
-        <v>159</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D68" t="s">
-        <v>142</v>
-      </c>
-      <c r="E68" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
-        <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F69" s="2"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="D70" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="E70" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="5">
-        <f t="shared" si="2"/>
+      <c r="A71" s="2">
+        <f>ROW()-1</f>
         <v>70</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="E71" s="5" t="s">
+      <c r="B71" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F71" s="5"/>
+      <c r="F71" s="2"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D72" t="s">
         <v>73</v>
@@ -2801,168 +2808,166 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <f t="shared" si="2"/>
+      <c r="A73" s="5">
+        <f>ROW()-1</f>
         <v>72</v>
       </c>
-      <c r="B73" t="s">
-        <v>153</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D73" t="s">
-        <v>157</v>
-      </c>
-      <c r="E73" t="s">
+      <c r="B73" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E73" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="5">
-        <f t="shared" si="2"/>
+      <c r="A74">
+        <f>ROW()-1</f>
         <v>73</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E74" s="5" t="s">
+      <c r="B74" t="s">
+        <v>128</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D74" t="s">
+        <v>73</v>
+      </c>
+      <c r="E74" t="s">
         <v>16</v>
-      </c>
-      <c r="F74" s="5"/>
-      <c r="G74" s="4" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="D75" t="s">
-        <v>73</v>
+        <v>157</v>
       </c>
       <c r="E75" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <f t="shared" si="2"/>
+      <c r="A76" s="5">
+        <f>ROW()-1</f>
         <v>75</v>
       </c>
-      <c r="B76" t="s">
-        <v>207</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D76" t="s">
-        <v>173</v>
-      </c>
-      <c r="E76" t="s">
+      <c r="B76" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E76" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F76" t="s">
-        <v>37</v>
+      <c r="F76" s="5"/>
+      <c r="G76" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="5">
-        <f t="shared" si="2"/>
+      <c r="A77">
+        <f>ROW()-1</f>
         <v>76</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" t="s">
+        <v>187</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D77" t="s">
+        <v>73</v>
+      </c>
+      <c r="E77" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="5">
+        <f>ROW()-1</f>
+        <v>77</v>
+      </c>
+      <c r="B78" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C78" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D78" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E78" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F77" s="5"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <f t="shared" si="2"/>
-        <v>77</v>
-      </c>
-      <c r="B78" t="s">
-        <v>35</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D78" t="s">
-        <v>31</v>
-      </c>
-      <c r="E78" t="s">
-        <v>15</v>
-      </c>
+      <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>149</v>
+        <v>35</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>150</v>
+        <v>61</v>
       </c>
       <c r="D79" t="s">
-        <v>168</v>
+        <v>31</v>
       </c>
       <c r="E79" t="s">
         <v>15</v>
       </c>
-      <c r="G79" s="4"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>149</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D80" t="s">
+        <v>168</v>
+      </c>
+      <c r="E80" t="s">
+        <v>15</v>
+      </c>
+      <c r="G80" s="4"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <f>ROW()-1</f>
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
         <v>113</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="D80" t="s">
-        <v>73</v>
-      </c>
-      <c r="E80" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <f t="shared" si="2"/>
-        <v>80</v>
-      </c>
-      <c r="B81" t="s">
-        <v>105</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="D81" t="s">
         <v>73</v>
@@ -2971,16 +2976,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D82" t="s">
         <v>73</v>
@@ -2989,30 +2994,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D83" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="E83" t="s">
         <v>15</v>
       </c>
-      <c r="F83" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>83</v>
       </c>
       <c r="B84" t="s">
@@ -3028,9 +3030,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>84</v>
       </c>
       <c r="B85" t="s">
@@ -3046,9 +3048,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>85</v>
       </c>
       <c r="B86" t="s">
@@ -3064,9 +3066,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>86</v>
       </c>
       <c r="B87" t="s">
@@ -3082,9 +3084,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>87</v>
       </c>
       <c r="B88" t="s">
@@ -3507,23 +3509,23 @@
     <hyperlink ref="C10" r:id="rId3" xr:uid="{360E041F-B0DD-4BBB-99F0-FEC11C74DF66}"/>
     <hyperlink ref="C8" r:id="rId4" xr:uid="{46F9E010-CBE8-4A2E-9C23-1ED4BB1B1F4E}"/>
     <hyperlink ref="C13" r:id="rId5" xr:uid="{25A28752-23E4-47D8-A121-5D1EA00837E8}"/>
-    <hyperlink ref="C78" r:id="rId6" xr:uid="{3D1DAB51-3975-4C63-8024-DE42B1A10551}"/>
-    <hyperlink ref="C61" r:id="rId7" xr:uid="{A88D270B-DD4D-4B26-B375-EB9E13EFB360}"/>
+    <hyperlink ref="C79" r:id="rId6" xr:uid="{3D1DAB51-3975-4C63-8024-DE42B1A10551}"/>
+    <hyperlink ref="C64" r:id="rId7" xr:uid="{A88D270B-DD4D-4B26-B375-EB9E13EFB360}"/>
     <hyperlink ref="C23" r:id="rId8" xr:uid="{8212B78A-A644-47F5-98D0-3B1A37A7D45E}"/>
     <hyperlink ref="C21" r:id="rId9" xr:uid="{7B89EAC2-F6B4-4EED-B8C9-86966B3540C8}"/>
     <hyperlink ref="C30" r:id="rId10" xr:uid="{2CF0B45E-39BB-45F0-B562-6F6A109D4AE6}"/>
     <hyperlink ref="C32" r:id="rId11" xr:uid="{F74243B0-9456-44C6-A8F8-7D4BC0097062}"/>
     <hyperlink ref="C33" r:id="rId12" xr:uid="{9E0E15EC-C7D6-453F-BB20-B4DC44E847C0}"/>
     <hyperlink ref="C12" r:id="rId13" xr:uid="{24945E02-001F-4EC2-B305-690B333CF5A7}"/>
-    <hyperlink ref="C67" r:id="rId14" xr:uid="{8EF49D9C-E60B-4173-BA06-3A5CB4948092}"/>
+    <hyperlink ref="C69" r:id="rId14" xr:uid="{8EF49D9C-E60B-4173-BA06-3A5CB4948092}"/>
     <hyperlink ref="C17" r:id="rId15" xr:uid="{EF98E54E-BA3E-4059-8787-256C26698DF2}"/>
     <hyperlink ref="C42" r:id="rId16" xr:uid="{AFC88B2F-E281-44A4-B755-AEEEDC044D4E}"/>
     <hyperlink ref="C44" r:id="rId17" xr:uid="{FCF2CE55-9407-4234-BD39-9931FA7929A1}"/>
-    <hyperlink ref="C69" r:id="rId18" xr:uid="{7170FF64-A78A-4745-A928-41A075FBEF23}"/>
+    <hyperlink ref="C71" r:id="rId18" xr:uid="{7170FF64-A78A-4745-A928-41A075FBEF23}"/>
     <hyperlink ref="C46" r:id="rId19" xr:uid="{2D20E59F-FD49-4561-9516-026EFCBAC280}"/>
     <hyperlink ref="C47" r:id="rId20" xr:uid="{E5A16AE2-EC0D-480F-92C4-628BBB8DF98B}"/>
     <hyperlink ref="C48" r:id="rId21" xr:uid="{0F5CC868-171D-4ACE-AACF-92490F0A235F}"/>
-    <hyperlink ref="C77" r:id="rId22" xr:uid="{31C5E189-B075-4CA9-8FDB-D7FC91DE6008}"/>
+    <hyperlink ref="C78" r:id="rId22" xr:uid="{31C5E189-B075-4CA9-8FDB-D7FC91DE6008}"/>
     <hyperlink ref="C49" r:id="rId23" xr:uid="{E7A6C803-C0F3-449E-8D52-3A4D7325CA42}"/>
     <hyperlink ref="C50" r:id="rId24" xr:uid="{1CF48142-F48F-4E72-871F-8481378F69C0}"/>
     <hyperlink ref="C6" r:id="rId25" xr:uid="{EB055FA2-9D2F-4517-AFA3-73B30C885722}"/>
@@ -3538,10 +3540,10 @@
     <hyperlink ref="C2" r:id="rId34" xr:uid="{1BF8D7CF-5169-4C51-8208-0334225B91B6}"/>
     <hyperlink ref="C3" r:id="rId35" xr:uid="{F4285FE3-4FDE-4007-9456-FF7142723C52}"/>
     <hyperlink ref="C4" r:id="rId36" xr:uid="{45D2EAC0-519A-4D4B-A91D-D076121D8E83}"/>
-    <hyperlink ref="C63" r:id="rId37" xr:uid="{A39EA5A2-4B4C-4792-88E5-3A106C4B97B4}"/>
-    <hyperlink ref="C70" r:id="rId38" xr:uid="{0060F7F0-2F01-4A54-A8A5-DA509EBDE87C}"/>
-    <hyperlink ref="C72" r:id="rId39" xr:uid="{A59214FE-37F1-4BCB-8FB8-D2425AE99834}"/>
-    <hyperlink ref="C74" r:id="rId40" xr:uid="{EE6108B9-B67A-4347-A1FF-7D6D16308B50}"/>
+    <hyperlink ref="C65" r:id="rId37" xr:uid="{A39EA5A2-4B4C-4792-88E5-3A106C4B97B4}"/>
+    <hyperlink ref="C72" r:id="rId38" xr:uid="{0060F7F0-2F01-4A54-A8A5-DA509EBDE87C}"/>
+    <hyperlink ref="C74" r:id="rId39" xr:uid="{A59214FE-37F1-4BCB-8FB8-D2425AE99834}"/>
+    <hyperlink ref="C76" r:id="rId40" xr:uid="{EE6108B9-B67A-4347-A1FF-7D6D16308B50}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>

</xml_diff>